<commit_message>
Add financial templates, configs, and update data files
Added balance sheet and income statement PDF templates, new FS mapping YAML config, and multiple .parquet artifacts for trial balance and general ledger data. Updated TB and GL Excel files and notebook to reflect new data structure and column types, including changes in row counts and type conversions for key columns.
</commit_message>
<xml_diff>
--- a/data/TB_2024.xlsx
+++ b/data/TB_2024.xlsx
@@ -5,16 +5,19 @@
   <workbookPr saveExternalLinkValues="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XA XUI - CVN\Documents\GitHub\Planning_agent\PY_PBC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/52ebbb93f357813a/10_Works/GitHub/Planning_Agent_NDD/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8BFFC3-FF41-44DA-A15C-5CC29DB30A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:1_{FA8BFFC3-FF41-44DA-A15C-5CC29DB30A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F0D202B-8B78-442A-A14B-5AADD8BFAEC7}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7784254E-2EFB-49AF-922A-1AA81A05D961}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7784254E-2EFB-49AF-922A-1AA81A05D961}"/>
   </bookViews>
   <sheets>
     <sheet name="GridViewExporter" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GridViewExporter!$A$1:$M$136</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="275">
   <si>
     <t>Số dư c.nợ</t>
   </si>
@@ -816,15 +819,6 @@
   </si>
   <si>
     <t>Chi phí thuế TNDN hiện hành</t>
-  </si>
-  <si>
-    <t>911</t>
-  </si>
-  <si>
-    <t>Xác định kết quả kinh doanh</t>
-  </si>
-  <si>
-    <t>Tổng cộng:</t>
   </si>
   <si>
     <t>Account No</t>
@@ -1012,6 +1006,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1337,65 +1335,65 @@
   <dimension ref="A1:M138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C63" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E71" sqref="E71"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="15.26953125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="15.28515625" style="1" customWidth="1"/>
     <col min="10" max="11" width="7" style="1" customWidth="1"/>
-    <col min="12" max="12" width="5.81640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="8.1796875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="5.85546875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="6" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>274</v>
-      </c>
       <c r="M1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1403,7 +1401,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D2" s="3">
         <v>6605748426</v>
@@ -1418,7 +1416,9 @@
       <c r="H2" s="3">
         <v>6270753793</v>
       </c>
-      <c r="I2" s="3"/>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
       <c r="J2" s="1">
         <v>1</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D3" s="3">
         <v>897868646</v>
@@ -1455,7 +1455,9 @@
       <c r="H3" s="3">
         <v>1733695818</v>
       </c>
-      <c r="I3" s="3"/>
+      <c r="I3" s="3">
+        <v>0</v>
+      </c>
       <c r="J3" s="1">
         <v>0</v>
       </c>
@@ -1469,7 +1471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1477,7 +1479,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D4" s="3">
         <v>897868646</v>
@@ -1492,7 +1494,9 @@
       <c r="H4" s="3">
         <v>1733695818</v>
       </c>
-      <c r="I4" s="3"/>
+      <c r="I4" s="3">
+        <v>0</v>
+      </c>
       <c r="J4" s="1">
         <v>0</v>
       </c>
@@ -1506,7 +1510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1514,7 +1518,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D5" s="3">
         <v>5707879780</v>
@@ -1529,7 +1533,9 @@
       <c r="H5" s="3">
         <v>4537057975</v>
       </c>
-      <c r="I5" s="3"/>
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
       <c r="J5" s="1">
         <v>0</v>
       </c>
@@ -1543,7 +1549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1551,7 +1557,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D6" s="3">
         <v>5707879780</v>
@@ -1566,7 +1572,9 @@
       <c r="H6" s="3">
         <v>4537057975</v>
       </c>
-      <c r="I6" s="3"/>
+      <c r="I6" s="3">
+        <v>0</v>
+      </c>
       <c r="J6" s="1">
         <v>0</v>
       </c>
@@ -1580,7 +1588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1588,7 +1596,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -1598,8 +1606,12 @@
       <c r="G7" s="3">
         <v>834790638</v>
       </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
       <c r="J7" s="1">
         <v>1</v>
       </c>
@@ -1613,7 +1625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1621,7 +1633,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -1631,8 +1643,12 @@
       <c r="G8" s="3">
         <v>834790638</v>
       </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0</v>
+      </c>
       <c r="J8" s="1">
         <v>0</v>
       </c>
@@ -1646,7 +1662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1654,7 +1670,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D9" s="3">
         <v>706266798</v>
@@ -1669,7 +1685,9 @@
       <c r="H9" s="3">
         <v>787548208</v>
       </c>
-      <c r="I9" s="3"/>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
       <c r="J9" s="1">
         <v>1</v>
       </c>
@@ -1683,7 +1701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1691,7 +1709,7 @@
         <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D10" s="3">
         <v>706266798</v>
@@ -1706,7 +1724,9 @@
       <c r="H10" s="3">
         <v>787548208</v>
       </c>
-      <c r="I10" s="3"/>
+      <c r="I10" s="3">
+        <v>0</v>
+      </c>
       <c r="J10" s="1">
         <v>0</v>
       </c>
@@ -1720,7 +1740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1728,7 +1748,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D11" s="3">
         <v>706266798</v>
@@ -1743,7 +1763,9 @@
       <c r="H11" s="3">
         <v>787548208</v>
       </c>
-      <c r="I11" s="3"/>
+      <c r="I11" s="3">
+        <v>0</v>
+      </c>
       <c r="J11" s="1">
         <v>0</v>
       </c>
@@ -1757,7 +1779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -1765,7 +1787,7 @@
         <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D12" s="3">
         <v>124047295</v>
@@ -1777,8 +1799,12 @@
       <c r="G12" s="3">
         <v>725251159</v>
       </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0</v>
+      </c>
       <c r="J12" s="1">
         <v>1</v>
       </c>
@@ -1792,7 +1818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -1800,7 +1826,7 @@
         <v>24</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D13" s="3">
         <v>124047295</v>
@@ -1812,8 +1838,12 @@
       <c r="G13" s="3">
         <v>725251159</v>
       </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0</v>
+      </c>
       <c r="J13" s="1">
         <v>0</v>
       </c>
@@ -1827,7 +1857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1835,7 +1865,7 @@
         <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -1845,8 +1875,12 @@
       <c r="G14" s="3">
         <v>169643637</v>
       </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0</v>
+      </c>
       <c r="J14" s="1">
         <v>0</v>
       </c>
@@ -1860,7 +1894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1868,7 +1902,7 @@
         <v>28</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D15" s="3">
         <v>124047295</v>
@@ -1880,8 +1914,12 @@
       <c r="G15" s="3">
         <v>555607522</v>
       </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0</v>
+      </c>
       <c r="J15" s="1">
         <v>0</v>
       </c>
@@ -1895,7 +1933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -1903,7 +1941,7 @@
         <v>30</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D16" s="3">
         <v>257292807</v>
@@ -1918,7 +1956,9 @@
       <c r="H16" s="3">
         <v>655664226</v>
       </c>
-      <c r="I16" s="3"/>
+      <c r="I16" s="3">
+        <v>0</v>
+      </c>
       <c r="J16" s="1">
         <v>1</v>
       </c>
@@ -1932,7 +1972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
@@ -1940,7 +1980,7 @@
         <v>30</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D17" s="3">
         <v>257292807</v>
@@ -1955,7 +1995,9 @@
       <c r="H17" s="3">
         <v>655664226</v>
       </c>
-      <c r="I17" s="3"/>
+      <c r="I17" s="3">
+        <v>0</v>
+      </c>
       <c r="J17" s="1">
         <v>0</v>
       </c>
@@ -1969,7 +2011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -1977,7 +2019,7 @@
         <v>33</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D18" s="3">
         <v>257292807</v>
@@ -1992,7 +2034,9 @@
       <c r="H18" s="3">
         <v>655664226</v>
       </c>
-      <c r="I18" s="3"/>
+      <c r="I18" s="3">
+        <v>0</v>
+      </c>
       <c r="J18" s="1">
         <v>0</v>
       </c>
@@ -2006,7 +2050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -2014,7 +2058,7 @@
         <v>35</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -2027,7 +2071,9 @@
       <c r="H19" s="3">
         <v>52850560</v>
       </c>
-      <c r="I19" s="3"/>
+      <c r="I19" s="3">
+        <v>0</v>
+      </c>
       <c r="J19" s="1">
         <v>0</v>
       </c>
@@ -2041,7 +2087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -2049,7 +2095,7 @@
         <v>33</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D20" s="3">
         <v>257292807</v>
@@ -2064,7 +2110,9 @@
       <c r="H20" s="3">
         <v>602813666</v>
       </c>
-      <c r="I20" s="3"/>
+      <c r="I20" s="3">
+        <v>0</v>
+      </c>
       <c r="J20" s="1">
         <v>0</v>
       </c>
@@ -2078,7 +2126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>37</v>
       </c>
@@ -2086,7 +2134,7 @@
         <v>38</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D21" s="3">
         <v>123228000</v>
@@ -2101,7 +2149,9 @@
       <c r="H21" s="3">
         <v>335576938</v>
       </c>
-      <c r="I21" s="3"/>
+      <c r="I21" s="3">
+        <v>0</v>
+      </c>
       <c r="J21" s="1">
         <v>1</v>
       </c>
@@ -2115,7 +2165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>39</v>
       </c>
@@ -2123,7 +2173,7 @@
         <v>40</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -2133,8 +2183,12 @@
       <c r="G22" s="3">
         <v>590137877</v>
       </c>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
+      <c r="H22" s="3">
+        <v>0</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0</v>
+      </c>
       <c r="J22" s="1">
         <v>1</v>
       </c>
@@ -2148,7 +2202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
@@ -2156,7 +2210,7 @@
         <v>42</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -2166,8 +2220,12 @@
       <c r="G23" s="3">
         <v>590137877</v>
       </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+      <c r="H23" s="3">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0</v>
+      </c>
       <c r="J23" s="1">
         <v>0</v>
       </c>
@@ -2181,7 +2239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>43</v>
       </c>
@@ -2189,7 +2247,7 @@
         <v>44</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -2199,8 +2257,12 @@
       <c r="G24" s="3">
         <v>4762403069</v>
       </c>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0</v>
+      </c>
       <c r="J24" s="1">
         <v>1</v>
       </c>
@@ -2214,7 +2276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>45</v>
       </c>
@@ -2222,7 +2284,7 @@
         <v>46</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -2232,8 +2294,12 @@
       <c r="G25" s="3">
         <v>4762403069</v>
       </c>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
+      <c r="H25" s="3">
+        <v>0</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0</v>
+      </c>
       <c r="J25" s="1">
         <v>0</v>
       </c>
@@ -2247,7 +2313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>47</v>
       </c>
@@ -2255,7 +2321,7 @@
         <v>48</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D26" s="3">
         <v>39320000</v>
@@ -2266,7 +2332,9 @@
       <c r="H26" s="3">
         <v>39320000</v>
       </c>
-      <c r="I26" s="3"/>
+      <c r="I26" s="3">
+        <v>0</v>
+      </c>
       <c r="J26" s="1">
         <v>1</v>
       </c>
@@ -2280,7 +2348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>49</v>
       </c>
@@ -2288,7 +2356,7 @@
         <v>50</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D27" s="3">
         <v>39320000</v>
@@ -2299,7 +2367,9 @@
       <c r="H27" s="3">
         <v>39320000</v>
       </c>
-      <c r="I27" s="3"/>
+      <c r="I27" s="3">
+        <v>0</v>
+      </c>
       <c r="J27" s="1">
         <v>0</v>
       </c>
@@ -2313,7 +2383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>51</v>
       </c>
@@ -2321,7 +2391,7 @@
         <v>52</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3">
@@ -2333,7 +2403,9 @@
       <c r="G28" s="3">
         <v>9829992</v>
       </c>
-      <c r="H28" s="3"/>
+      <c r="H28" s="3">
+        <v>0</v>
+      </c>
       <c r="I28" s="3">
         <v>28452366</v>
       </c>
@@ -2350,7 +2422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>53</v>
       </c>
@@ -2358,7 +2430,7 @@
         <v>54</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3">
@@ -2370,7 +2442,9 @@
       <c r="G29" s="3">
         <v>9829992</v>
       </c>
-      <c r="H29" s="3"/>
+      <c r="H29" s="3">
+        <v>0</v>
+      </c>
       <c r="I29" s="3">
         <v>28452366</v>
       </c>
@@ -2387,7 +2461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>55</v>
       </c>
@@ -2395,7 +2469,7 @@
         <v>56</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3">
@@ -2407,7 +2481,9 @@
       <c r="G30" s="3">
         <v>9829992</v>
       </c>
-      <c r="H30" s="3"/>
+      <c r="H30" s="3">
+        <v>0</v>
+      </c>
       <c r="I30" s="3">
         <v>28452366</v>
       </c>
@@ -2424,7 +2500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>57</v>
       </c>
@@ -2432,7 +2508,7 @@
         <v>58</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D31" s="3">
         <v>117685490</v>
@@ -2447,7 +2523,9 @@
       <c r="H31" s="3">
         <v>149686568</v>
       </c>
-      <c r="I31" s="3"/>
+      <c r="I31" s="3">
+        <v>0</v>
+      </c>
       <c r="J31" s="1">
         <v>1</v>
       </c>
@@ -2461,7 +2539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>59</v>
       </c>
@@ -2469,7 +2547,7 @@
         <v>60</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D32" s="3">
         <v>101595093</v>
@@ -2484,7 +2562,9 @@
       <c r="H32" s="3">
         <v>118340962</v>
       </c>
-      <c r="I32" s="3"/>
+      <c r="I32" s="3">
+        <v>0</v>
+      </c>
       <c r="J32" s="1">
         <v>0</v>
       </c>
@@ -2498,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
@@ -2506,7 +2586,7 @@
         <v>62</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -2516,8 +2596,12 @@
       <c r="G33" s="3">
         <v>10890000</v>
       </c>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
+      <c r="H33" s="3">
+        <v>0</v>
+      </c>
+      <c r="I33" s="3">
+        <v>0</v>
+      </c>
       <c r="J33" s="1">
         <v>0</v>
       </c>
@@ -2531,7 +2615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>63</v>
       </c>
@@ -2539,7 +2623,7 @@
         <v>64</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D34" s="3">
         <v>101595093</v>
@@ -2554,7 +2638,9 @@
       <c r="H34" s="3">
         <v>118340962</v>
       </c>
-      <c r="I34" s="3"/>
+      <c r="I34" s="3">
+        <v>0</v>
+      </c>
       <c r="J34" s="1">
         <v>0</v>
       </c>
@@ -2568,7 +2654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>65</v>
       </c>
@@ -2576,7 +2662,7 @@
         <v>66</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D35" s="3">
         <v>16090397</v>
@@ -2591,7 +2677,9 @@
       <c r="H35" s="3">
         <v>31345606</v>
       </c>
-      <c r="I35" s="3"/>
+      <c r="I35" s="3">
+        <v>0</v>
+      </c>
       <c r="J35" s="1">
         <v>0</v>
       </c>
@@ -2605,7 +2693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>67</v>
       </c>
@@ -2613,7 +2701,7 @@
         <v>68</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D36" s="3">
         <v>10549745</v>
@@ -2628,7 +2716,9 @@
       <c r="H36" s="3">
         <v>21962129</v>
       </c>
-      <c r="I36" s="3"/>
+      <c r="I36" s="3">
+        <v>0</v>
+      </c>
       <c r="J36" s="1">
         <v>0</v>
       </c>
@@ -2642,7 +2732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>69</v>
       </c>
@@ -2650,7 +2740,7 @@
         <v>70</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D37" s="3">
         <v>5540652</v>
@@ -2665,7 +2755,9 @@
       <c r="H37" s="3">
         <v>9383477</v>
       </c>
-      <c r="I37" s="3"/>
+      <c r="I37" s="3">
+        <v>0</v>
+      </c>
       <c r="J37" s="1">
         <v>0</v>
       </c>
@@ -2679,7 +2771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>71</v>
       </c>
@@ -2687,7 +2779,7 @@
         <v>72</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D38" s="3">
         <v>148099200</v>
@@ -2698,7 +2790,9 @@
       <c r="H38" s="3">
         <v>148099200</v>
       </c>
-      <c r="I38" s="3"/>
+      <c r="I38" s="3">
+        <v>0</v>
+      </c>
       <c r="J38" s="1">
         <v>1</v>
       </c>
@@ -2712,7 +2806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>73</v>
       </c>
@@ -2720,7 +2814,7 @@
         <v>74</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D39" s="3">
         <v>148099200</v>
@@ -2731,7 +2825,9 @@
       <c r="H39" s="3">
         <v>148099200</v>
       </c>
-      <c r="I39" s="3"/>
+      <c r="I39" s="3">
+        <v>0</v>
+      </c>
       <c r="J39" s="1">
         <v>0</v>
       </c>
@@ -2745,7 +2841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>75</v>
       </c>
@@ -2753,7 +2849,7 @@
         <v>76</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D40" s="3">
         <v>91360</v>
@@ -2786,7 +2882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>77</v>
       </c>
@@ -2794,7 +2890,7 @@
         <v>78</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D41" s="3">
         <v>91360</v>
@@ -2827,7 +2923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>79</v>
       </c>
@@ -2835,7 +2931,7 @@
         <v>80</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D42" s="3">
         <v>91360</v>
@@ -2868,7 +2964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>81</v>
       </c>
@@ -2876,7 +2972,7 @@
         <v>82</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" s="3">
@@ -2888,7 +2984,9 @@
       <c r="G43" s="3">
         <v>4393777280</v>
       </c>
-      <c r="H43" s="3"/>
+      <c r="H43" s="3">
+        <v>0</v>
+      </c>
       <c r="I43" s="3">
         <v>323313453</v>
       </c>
@@ -2905,7 +3003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>83</v>
       </c>
@@ -2913,7 +3011,7 @@
         <v>84</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" s="3">
@@ -2925,7 +3023,9 @@
       <c r="G44" s="3">
         <v>2330478004</v>
       </c>
-      <c r="H44" s="3"/>
+      <c r="H44" s="3">
+        <v>0</v>
+      </c>
       <c r="I44" s="3">
         <v>20709338</v>
       </c>
@@ -2942,7 +3042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>85</v>
       </c>
@@ -2950,7 +3050,7 @@
         <v>86</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
@@ -2960,7 +3060,9 @@
       <c r="G45" s="3">
         <v>1089985368</v>
       </c>
-      <c r="H45" s="3"/>
+      <c r="H45" s="3">
+        <v>0</v>
+      </c>
       <c r="I45" s="3">
         <v>17355966</v>
       </c>
@@ -2977,7 +3079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>87</v>
       </c>
@@ -2985,7 +3087,7 @@
         <v>88</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
@@ -2995,7 +3097,9 @@
       <c r="G46" s="3">
         <v>742607125</v>
       </c>
-      <c r="H46" s="3"/>
+      <c r="H46" s="3">
+        <v>0</v>
+      </c>
       <c r="I46" s="3">
         <v>17355966</v>
       </c>
@@ -3012,7 +3116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>89</v>
       </c>
@@ -3020,7 +3124,7 @@
         <v>90</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
@@ -3030,7 +3134,9 @@
       <c r="G47" s="3">
         <v>742607125</v>
       </c>
-      <c r="H47" s="3"/>
+      <c r="H47" s="3">
+        <v>0</v>
+      </c>
       <c r="I47" s="3">
         <v>17355966</v>
       </c>
@@ -3047,7 +3153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>91</v>
       </c>
@@ -3055,7 +3161,7 @@
         <v>92</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
@@ -3065,8 +3171,12 @@
       <c r="G48" s="3">
         <v>347378243</v>
       </c>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
+      <c r="H48" s="3">
+        <v>0</v>
+      </c>
+      <c r="I48" s="3">
+        <v>0</v>
+      </c>
       <c r="J48" s="1">
         <v>0</v>
       </c>
@@ -3080,7 +3190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>93</v>
       </c>
@@ -3088,7 +3198,7 @@
         <v>94</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
@@ -3098,8 +3208,12 @@
       <c r="G49" s="3">
         <v>10640416</v>
       </c>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
+      <c r="H49" s="3">
+        <v>0</v>
+      </c>
+      <c r="I49" s="3">
+        <v>0</v>
+      </c>
       <c r="J49" s="1">
         <v>0</v>
       </c>
@@ -3113,7 +3227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>95</v>
       </c>
@@ -3121,7 +3235,7 @@
         <v>96</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
@@ -3131,8 +3245,12 @@
       <c r="G50" s="3">
         <v>5295224</v>
       </c>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
+      <c r="H50" s="3">
+        <v>0</v>
+      </c>
+      <c r="I50" s="3">
+        <v>0</v>
+      </c>
       <c r="J50" s="1">
         <v>0</v>
       </c>
@@ -3146,7 +3264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>97</v>
       </c>
@@ -3154,7 +3272,7 @@
         <v>98</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
@@ -3164,8 +3282,12 @@
       <c r="G51" s="3">
         <v>5345192</v>
       </c>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
+      <c r="H51" s="3">
+        <v>0</v>
+      </c>
+      <c r="I51" s="3">
+        <v>0</v>
+      </c>
       <c r="J51" s="1">
         <v>0</v>
       </c>
@@ -3179,7 +3301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>99</v>
       </c>
@@ -3187,7 +3309,7 @@
         <v>100</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
@@ -3197,8 +3319,12 @@
       <c r="G52" s="3">
         <v>123407221</v>
       </c>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
+      <c r="H52" s="3">
+        <v>0</v>
+      </c>
+      <c r="I52" s="3">
+        <v>0</v>
+      </c>
       <c r="J52" s="1">
         <v>0</v>
       </c>
@@ -3212,7 +3338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>101</v>
       </c>
@@ -3220,7 +3346,7 @@
         <v>102</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D53" s="3"/>
       <c r="E53" s="3">
@@ -3232,7 +3358,9 @@
       <c r="G53" s="3">
         <v>1093319057</v>
       </c>
-      <c r="H53" s="3"/>
+      <c r="H53" s="3">
+        <v>0</v>
+      </c>
       <c r="I53" s="3">
         <v>3353372</v>
       </c>
@@ -3249,7 +3377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>103</v>
       </c>
@@ -3257,7 +3385,7 @@
         <v>104</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
@@ -3267,8 +3395,12 @@
       <c r="G54" s="3">
         <v>9485942</v>
       </c>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
+      <c r="H54" s="3">
+        <v>0</v>
+      </c>
+      <c r="I54" s="3">
+        <v>0</v>
+      </c>
       <c r="J54" s="1">
         <v>0</v>
       </c>
@@ -3282,7 +3414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>105</v>
       </c>
@@ -3290,7 +3422,7 @@
         <v>106</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
@@ -3300,8 +3432,12 @@
       <c r="G55" s="3">
         <v>9485942</v>
       </c>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
+      <c r="H55" s="3">
+        <v>0</v>
+      </c>
+      <c r="I55" s="3">
+        <v>0</v>
+      </c>
       <c r="J55" s="1">
         <v>0</v>
       </c>
@@ -3315,7 +3451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>107</v>
       </c>
@@ -3323,7 +3459,7 @@
         <v>108</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
@@ -3333,8 +3469,12 @@
       <c r="G56" s="3">
         <v>3640000</v>
       </c>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
+      <c r="H56" s="3">
+        <v>0</v>
+      </c>
+      <c r="I56" s="3">
+        <v>0</v>
+      </c>
       <c r="J56" s="1">
         <v>0</v>
       </c>
@@ -3348,7 +3488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>109</v>
       </c>
@@ -3356,7 +3496,7 @@
         <v>110</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
@@ -3366,8 +3506,12 @@
       <c r="G57" s="3">
         <v>3640000</v>
       </c>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
+      <c r="H57" s="3">
+        <v>0</v>
+      </c>
+      <c r="I57" s="3">
+        <v>0</v>
+      </c>
       <c r="J57" s="1">
         <v>0</v>
       </c>
@@ -3381,7 +3525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>111</v>
       </c>
@@ -3389,7 +3533,7 @@
         <v>112</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D58" s="3"/>
       <c r="E58" s="3">
@@ -3401,7 +3545,9 @@
       <c r="G58" s="3">
         <v>1540017016</v>
       </c>
-      <c r="H58" s="3"/>
+      <c r="H58" s="3">
+        <v>0</v>
+      </c>
       <c r="I58" s="3">
         <v>48145085</v>
       </c>
@@ -3418,7 +3564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>113</v>
       </c>
@@ -3426,7 +3572,7 @@
         <v>112</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D59" s="3"/>
       <c r="E59" s="3">
@@ -3438,7 +3584,9 @@
       <c r="G59" s="3">
         <v>1540017016</v>
       </c>
-      <c r="H59" s="3"/>
+      <c r="H59" s="3">
+        <v>0</v>
+      </c>
       <c r="I59" s="3">
         <v>48145085</v>
       </c>
@@ -3455,7 +3603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>114</v>
       </c>
@@ -3463,7 +3611,7 @@
         <v>115</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D60" s="3"/>
       <c r="E60" s="3">
@@ -3475,7 +3623,9 @@
       <c r="G60" s="3">
         <v>567649822</v>
       </c>
-      <c r="H60" s="3"/>
+      <c r="H60" s="3">
+        <v>0</v>
+      </c>
       <c r="I60" s="3">
         <v>48145085</v>
       </c>
@@ -3492,7 +3642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>116</v>
       </c>
@@ -3500,7 +3650,7 @@
         <v>117</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
@@ -3510,8 +3660,12 @@
       <c r="G61" s="3">
         <v>972367194</v>
       </c>
-      <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
+      <c r="H61" s="3">
+        <v>0</v>
+      </c>
+      <c r="I61" s="3">
+        <v>0</v>
+      </c>
       <c r="J61" s="1">
         <v>0</v>
       </c>
@@ -3525,7 +3679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>118</v>
       </c>
@@ -3533,7 +3687,7 @@
         <v>119</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D62" s="3"/>
       <c r="E62" s="3">
@@ -3545,7 +3699,9 @@
       <c r="G62" s="3">
         <v>212615391</v>
       </c>
-      <c r="H62" s="3"/>
+      <c r="H62" s="3">
+        <v>0</v>
+      </c>
       <c r="I62" s="3">
         <v>419095788</v>
       </c>
@@ -3562,7 +3718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>120</v>
       </c>
@@ -3570,7 +3726,7 @@
         <v>121</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3">
@@ -3582,7 +3738,9 @@
       <c r="G63" s="3">
         <v>1070178636</v>
       </c>
-      <c r="H63" s="3"/>
+      <c r="H63" s="3">
+        <v>0</v>
+      </c>
       <c r="I63" s="3">
         <v>46657293</v>
       </c>
@@ -3599,7 +3757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>122</v>
       </c>
@@ -3607,7 +3765,7 @@
         <v>123</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -3617,8 +3775,12 @@
       <c r="G64" s="3">
         <v>9302858</v>
       </c>
-      <c r="H64" s="3"/>
-      <c r="I64" s="3"/>
+      <c r="H64" s="3">
+        <v>0</v>
+      </c>
+      <c r="I64" s="3">
+        <v>0</v>
+      </c>
       <c r="J64" s="1">
         <v>0</v>
       </c>
@@ -3632,7 +3794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>124</v>
       </c>
@@ -3640,7 +3802,7 @@
         <v>125</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
@@ -3650,8 +3812,12 @@
       <c r="G65" s="3">
         <v>118611455</v>
       </c>
-      <c r="H65" s="3"/>
-      <c r="I65" s="3"/>
+      <c r="H65" s="3">
+        <v>0</v>
+      </c>
+      <c r="I65" s="3">
+        <v>0</v>
+      </c>
       <c r="J65" s="1">
         <v>0</v>
       </c>
@@ -3665,7 +3831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>126</v>
       </c>
@@ -3673,7 +3839,7 @@
         <v>127</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
@@ -3683,8 +3849,12 @@
       <c r="G66" s="3">
         <v>20931432</v>
       </c>
-      <c r="H66" s="3"/>
-      <c r="I66" s="3"/>
+      <c r="H66" s="3">
+        <v>0</v>
+      </c>
+      <c r="I66" s="3">
+        <v>0</v>
+      </c>
       <c r="J66" s="1">
         <v>0</v>
       </c>
@@ -3698,7 +3868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>128</v>
       </c>
@@ -3706,7 +3876,7 @@
         <v>129</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
@@ -3716,8 +3886,12 @@
       <c r="G67" s="3">
         <v>9302864</v>
       </c>
-      <c r="H67" s="3"/>
-      <c r="I67" s="3"/>
+      <c r="H67" s="3">
+        <v>0</v>
+      </c>
+      <c r="I67" s="3">
+        <v>0</v>
+      </c>
       <c r="J67" s="1">
         <v>0</v>
       </c>
@@ -3731,7 +3905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>130</v>
       </c>
@@ -3739,7 +3913,7 @@
         <v>121</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D68" s="3"/>
       <c r="E68" s="3">
@@ -3751,7 +3925,9 @@
       <c r="G68" s="3">
         <v>912030027</v>
       </c>
-      <c r="H68" s="3"/>
+      <c r="H68" s="3">
+        <v>0</v>
+      </c>
       <c r="I68" s="3">
         <v>46657293</v>
       </c>
@@ -3768,7 +3944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>131</v>
       </c>
@@ -3776,7 +3952,7 @@
         <v>132</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="3">
@@ -3788,7 +3964,9 @@
       <c r="G69" s="3">
         <v>912030027</v>
       </c>
-      <c r="H69" s="3"/>
+      <c r="H69" s="3">
+        <v>0</v>
+      </c>
       <c r="I69" s="3">
         <v>46657293</v>
       </c>
@@ -3805,7 +3983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>133</v>
       </c>
@@ -3813,7 +3991,7 @@
         <v>132</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D70" s="3"/>
       <c r="E70" s="3">
@@ -3825,7 +4003,9 @@
       <c r="G70" s="3">
         <v>912030027</v>
       </c>
-      <c r="H70" s="3"/>
+      <c r="H70" s="3">
+        <v>0</v>
+      </c>
       <c r="I70" s="3">
         <v>46657293</v>
       </c>
@@ -3842,7 +4022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>134</v>
       </c>
@@ -3850,7 +4030,7 @@
         <v>135</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D71" s="3"/>
       <c r="E71" s="3">
@@ -3858,7 +4038,9 @@
       </c>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
-      <c r="H71" s="3"/>
+      <c r="H71" s="3">
+        <v>0</v>
+      </c>
       <c r="I71" s="3">
         <v>13746000000</v>
       </c>
@@ -3875,7 +4057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>136</v>
       </c>
@@ -3883,7 +4065,7 @@
         <v>137</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D72" s="3"/>
       <c r="E72" s="3">
@@ -3891,7 +4073,9 @@
       </c>
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
-      <c r="H72" s="3"/>
+      <c r="H72" s="3">
+        <v>0</v>
+      </c>
       <c r="I72" s="3">
         <v>13746000000</v>
       </c>
@@ -3908,7 +4092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>138</v>
       </c>
@@ -3916,7 +4100,7 @@
         <v>139</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
@@ -3926,8 +4110,12 @@
       <c r="G73" s="3">
         <v>76685</v>
       </c>
-      <c r="H73" s="3"/>
-      <c r="I73" s="3"/>
+      <c r="H73" s="3">
+        <v>0</v>
+      </c>
+      <c r="I73" s="3">
+        <v>0</v>
+      </c>
       <c r="J73" s="1">
         <v>1</v>
       </c>
@@ -3941,7 +4129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>140</v>
       </c>
@@ -3949,7 +4137,7 @@
         <v>141</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
@@ -3959,8 +4147,12 @@
       <c r="G74" s="3">
         <v>76685</v>
       </c>
-      <c r="H74" s="3"/>
-      <c r="I74" s="3"/>
+      <c r="H74" s="3">
+        <v>0</v>
+      </c>
+      <c r="I74" s="3">
+        <v>0</v>
+      </c>
       <c r="J74" s="1">
         <v>0</v>
       </c>
@@ -3974,7 +4166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>142</v>
       </c>
@@ -3982,7 +4174,7 @@
         <v>143</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D75" s="3">
         <v>6290591391</v>
@@ -3997,7 +4189,9 @@
       <c r="H75" s="3">
         <v>6299797766</v>
       </c>
-      <c r="I75" s="3"/>
+      <c r="I75" s="3">
+        <v>0</v>
+      </c>
       <c r="J75" s="1">
         <v>1</v>
       </c>
@@ -4011,7 +4205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>144</v>
       </c>
@@ -4019,7 +4213,7 @@
         <v>145</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D76" s="3">
         <v>4171107126</v>
@@ -4032,7 +4226,9 @@
       <c r="H76" s="3">
         <v>6290591391</v>
       </c>
-      <c r="I76" s="3"/>
+      <c r="I76" s="3">
+        <v>0</v>
+      </c>
       <c r="J76" s="1">
         <v>0</v>
       </c>
@@ -4046,7 +4242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>146</v>
       </c>
@@ -4054,7 +4250,7 @@
         <v>147</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D77" s="3">
         <v>2119484265</v>
@@ -4069,7 +4265,9 @@
       <c r="H77" s="3">
         <v>9206375</v>
       </c>
-      <c r="I77" s="3"/>
+      <c r="I77" s="3">
+        <v>0</v>
+      </c>
       <c r="J77" s="1">
         <v>0</v>
       </c>
@@ -4083,7 +4281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>148</v>
       </c>
@@ -4091,11 +4289,13 @@
         <v>149</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
+      <c r="F78" s="3">
+        <v>0</v>
+      </c>
       <c r="G78" s="3">
         <v>0</v>
       </c>
@@ -4114,7 +4314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>150</v>
       </c>
@@ -4122,11 +4322,13 @@
         <v>151</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
+      <c r="F79" s="3">
+        <v>0</v>
+      </c>
       <c r="G79" s="3">
         <v>6421735813</v>
       </c>
@@ -4145,7 +4347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>152</v>
       </c>
@@ -4153,11 +4355,13 @@
         <v>153</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
+      <c r="F80" s="3">
+        <v>0</v>
+      </c>
       <c r="G80" s="3">
         <v>596942428</v>
       </c>
@@ -4176,7 +4380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>154</v>
       </c>
@@ -4184,11 +4388,13 @@
         <v>155</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
-      <c r="F81" s="3"/>
+      <c r="F81" s="3">
+        <v>0</v>
+      </c>
       <c r="G81" s="3">
         <v>784740170</v>
       </c>
@@ -4207,7 +4413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>156</v>
       </c>
@@ -4215,11 +4421,13 @@
         <v>157</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
-      <c r="F82" s="3"/>
+      <c r="F82" s="3">
+        <v>0</v>
+      </c>
       <c r="G82" s="3">
         <v>0</v>
       </c>
@@ -4238,7 +4446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>158</v>
       </c>
@@ -4246,11 +4454,13 @@
         <v>159</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
-      <c r="F83" s="3"/>
+      <c r="F83" s="3">
+        <v>0</v>
+      </c>
       <c r="G83" s="3">
         <v>997616</v>
       </c>
@@ -4269,7 +4479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>160</v>
       </c>
@@ -4277,11 +4487,13 @@
         <v>161</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
-      <c r="F84" s="3"/>
+      <c r="F84" s="3">
+        <v>0</v>
+      </c>
       <c r="G84" s="3">
         <v>154099165</v>
       </c>
@@ -4300,7 +4512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>162</v>
       </c>
@@ -4308,11 +4520,13 @@
         <v>163</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
-      <c r="F85" s="3"/>
+      <c r="F85" s="3">
+        <v>0</v>
+      </c>
       <c r="G85" s="3">
         <v>-26002382</v>
       </c>
@@ -4331,7 +4545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>168</v>
       </c>
@@ -4339,14 +4553,16 @@
         <v>169</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
       <c r="F86" s="3">
-        <v>0</v>
-      </c>
-      <c r="G86" s="3"/>
+        <v>5387434959</v>
+      </c>
+      <c r="G86" s="3">
+        <v>0</v>
+      </c>
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
       <c r="J86" s="1">
@@ -4362,7 +4578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>170</v>
       </c>
@@ -4370,14 +4586,16 @@
         <v>171</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
       <c r="F87" s="3">
         <v>4749752753</v>
       </c>
-      <c r="G87" s="3"/>
+      <c r="G87" s="3">
+        <v>0</v>
+      </c>
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
       <c r="J87" s="1">
@@ -4393,7 +4611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>172</v>
       </c>
@@ -4401,14 +4619,16 @@
         <v>173</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
       <c r="F88" s="3">
         <v>637682206</v>
       </c>
-      <c r="G88" s="3"/>
+      <c r="G88" s="3">
+        <v>0</v>
+      </c>
       <c r="H88" s="3"/>
       <c r="I88" s="3"/>
       <c r="J88" s="1">
@@ -4424,7 +4644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>174</v>
       </c>
@@ -4432,14 +4652,16 @@
         <v>175</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
       <c r="F89" s="3">
         <v>0</v>
       </c>
-      <c r="G89" s="3"/>
+      <c r="G89" s="3">
+        <v>0</v>
+      </c>
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
       <c r="J89" s="1">
@@ -4455,7 +4677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>176</v>
       </c>
@@ -4463,14 +4685,16 @@
         <v>177</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
       <c r="F90" s="3">
         <v>4853244</v>
       </c>
-      <c r="G90" s="3"/>
+      <c r="G90" s="3">
+        <v>0</v>
+      </c>
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
       <c r="J90" s="1">
@@ -4486,7 +4710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>178</v>
       </c>
@@ -4494,14 +4718,16 @@
         <v>179</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
       <c r="F91" s="3">
         <v>0</v>
       </c>
-      <c r="G91" s="3"/>
+      <c r="G91" s="3">
+        <v>0</v>
+      </c>
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
       <c r="J91" s="1">
@@ -4517,7 +4743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>180</v>
       </c>
@@ -4525,14 +4751,16 @@
         <v>181</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
       <c r="F92" s="3">
         <v>0</v>
       </c>
-      <c r="G92" s="3"/>
+      <c r="G92" s="3">
+        <v>0</v>
+      </c>
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
       <c r="J92" s="1">
@@ -4548,7 +4776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>182</v>
       </c>
@@ -4556,14 +4784,16 @@
         <v>183</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
       <c r="F93" s="3">
         <v>385354183</v>
       </c>
-      <c r="G93" s="3"/>
+      <c r="G93" s="3">
+        <v>0</v>
+      </c>
       <c r="H93" s="3"/>
       <c r="I93" s="3"/>
       <c r="J93" s="1">
@@ -4579,7 +4809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>184</v>
       </c>
@@ -4587,14 +4817,16 @@
         <v>185</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
       <c r="F94" s="3">
         <v>-653330658</v>
       </c>
-      <c r="G94" s="3"/>
+      <c r="G94" s="3">
+        <v>0</v>
+      </c>
       <c r="H94" s="3"/>
       <c r="I94" s="3"/>
       <c r="J94" s="1">
@@ -4610,7 +4842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>186</v>
       </c>
@@ -4618,14 +4850,16 @@
         <v>187</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
       <c r="F95" s="3">
         <v>85483250</v>
       </c>
-      <c r="G95" s="3"/>
+      <c r="G95" s="3">
+        <v>0</v>
+      </c>
       <c r="H95" s="3"/>
       <c r="I95" s="3"/>
       <c r="J95" s="1">
@@ -4641,7 +4875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>188</v>
       </c>
@@ -4649,14 +4883,16 @@
         <v>189</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
       <c r="F96" s="3">
         <v>341600000</v>
       </c>
-      <c r="G96" s="3"/>
+      <c r="G96" s="3">
+        <v>0</v>
+      </c>
       <c r="H96" s="3"/>
       <c r="I96" s="3"/>
       <c r="J96" s="1">
@@ -4672,7 +4908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>190</v>
       </c>
@@ -4680,14 +4916,16 @@
         <v>191</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
       <c r="F97" s="3">
         <v>537899390</v>
       </c>
-      <c r="G97" s="3"/>
+      <c r="G97" s="3">
+        <v>0</v>
+      </c>
       <c r="H97" s="3"/>
       <c r="I97" s="3"/>
       <c r="J97" s="1">
@@ -4703,7 +4941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>192</v>
       </c>
@@ -4711,14 +4949,16 @@
         <v>193</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D98" s="3"/>
       <c r="E98" s="3"/>
       <c r="F98" s="3">
         <v>99204446</v>
       </c>
-      <c r="G98" s="3"/>
+      <c r="G98" s="3">
+        <v>0</v>
+      </c>
       <c r="H98" s="3"/>
       <c r="I98" s="3"/>
       <c r="J98" s="1">
@@ -4734,7 +4974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>194</v>
       </c>
@@ -4742,14 +4982,16 @@
         <v>195</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
       <c r="F99" s="3">
         <v>0</v>
       </c>
-      <c r="G99" s="3"/>
+      <c r="G99" s="3">
+        <v>0</v>
+      </c>
       <c r="H99" s="3"/>
       <c r="I99" s="3"/>
       <c r="J99" s="1">
@@ -4765,7 +5007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>196</v>
       </c>
@@ -4773,14 +5015,16 @@
         <v>197</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
       <c r="F100" s="3">
         <v>4914996</v>
       </c>
-      <c r="G100" s="3"/>
+      <c r="G100" s="3">
+        <v>0</v>
+      </c>
       <c r="H100" s="3"/>
       <c r="I100" s="3"/>
       <c r="J100" s="1">
@@ -4796,7 +5040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>198</v>
       </c>
@@ -4804,14 +5048,16 @@
         <v>164</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
       <c r="F101" s="3">
         <v>0</v>
       </c>
-      <c r="G101" s="3"/>
+      <c r="G101" s="3">
+        <v>0</v>
+      </c>
       <c r="H101" s="3"/>
       <c r="I101" s="3"/>
       <c r="J101" s="1">
@@ -4827,7 +5073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>199</v>
       </c>
@@ -4835,14 +5081,16 @@
         <v>200</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
       <c r="F102" s="3">
         <v>243226195</v>
       </c>
-      <c r="G102" s="3"/>
+      <c r="G102" s="3">
+        <v>0</v>
+      </c>
       <c r="H102" s="3"/>
       <c r="I102" s="3"/>
       <c r="J102" s="1">
@@ -4858,7 +5106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>201</v>
       </c>
@@ -4866,14 +5114,16 @@
         <v>202</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>
       <c r="F103" s="3">
         <v>181834032</v>
       </c>
-      <c r="G103" s="3"/>
+      <c r="G103" s="3">
+        <v>0</v>
+      </c>
       <c r="H103" s="3"/>
       <c r="I103" s="3"/>
       <c r="J103" s="1">
@@ -4889,7 +5139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>203</v>
       </c>
@@ -4897,14 +5147,16 @@
         <v>204</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D104" s="3"/>
       <c r="E104" s="3"/>
       <c r="F104" s="3">
         <v>240187181</v>
       </c>
-      <c r="G104" s="3"/>
+      <c r="G104" s="3">
+        <v>0</v>
+      </c>
       <c r="H104" s="3"/>
       <c r="I104" s="3"/>
       <c r="J104" s="1">
@@ -4920,7 +5172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>205</v>
       </c>
@@ -4928,14 +5180,16 @@
         <v>206</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D105" s="3"/>
       <c r="E105" s="3"/>
       <c r="F105" s="3">
         <v>12330663</v>
       </c>
-      <c r="G105" s="3"/>
+      <c r="G105" s="3">
+        <v>0</v>
+      </c>
       <c r="H105" s="3"/>
       <c r="I105" s="3"/>
       <c r="J105" s="1">
@@ -4951,7 +5205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>207</v>
       </c>
@@ -4959,14 +5213,16 @@
         <v>208</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D106" s="3"/>
       <c r="E106" s="3"/>
       <c r="F106" s="3">
         <v>89308459</v>
       </c>
-      <c r="G106" s="3"/>
+      <c r="G106" s="3">
+        <v>0</v>
+      </c>
       <c r="H106" s="3"/>
       <c r="I106" s="3"/>
       <c r="J106" s="1">
@@ -4982,7 +5238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>209</v>
       </c>
@@ -4990,14 +5246,16 @@
         <v>166</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
       <c r="F107" s="3">
         <v>0</v>
       </c>
-      <c r="G107" s="3"/>
+      <c r="G107" s="3">
+        <v>0</v>
+      </c>
       <c r="H107" s="3"/>
       <c r="I107" s="3"/>
       <c r="J107" s="1">
@@ -5013,7 +5271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>210</v>
       </c>
@@ -5021,14 +5279,16 @@
         <v>167</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D108" s="3"/>
       <c r="E108" s="3"/>
       <c r="F108" s="3">
         <v>26630000</v>
       </c>
-      <c r="G108" s="3"/>
+      <c r="G108" s="3">
+        <v>0</v>
+      </c>
       <c r="H108" s="3"/>
       <c r="I108" s="3"/>
       <c r="J108" s="1">
@@ -5044,7 +5304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>211</v>
       </c>
@@ -5052,14 +5312,16 @@
         <v>212</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D109" s="3"/>
       <c r="E109" s="3"/>
       <c r="F109" s="3">
         <v>51973310</v>
       </c>
-      <c r="G109" s="3"/>
+      <c r="G109" s="3">
+        <v>0</v>
+      </c>
       <c r="H109" s="3"/>
       <c r="I109" s="3"/>
       <c r="J109" s="1">
@@ -5075,7 +5337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>213</v>
       </c>
@@ -5083,14 +5345,16 @@
         <v>214</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
       <c r="F110" s="3">
         <v>10341004</v>
       </c>
-      <c r="G110" s="3"/>
+      <c r="G110" s="3">
+        <v>0</v>
+      </c>
       <c r="H110" s="3"/>
       <c r="I110" s="3"/>
       <c r="J110" s="1">
@@ -5106,7 +5370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>215</v>
       </c>
@@ -5114,14 +5378,16 @@
         <v>216</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
       <c r="F111" s="3">
         <v>0</v>
       </c>
-      <c r="G111" s="3"/>
+      <c r="G111" s="3">
+        <v>0</v>
+      </c>
       <c r="H111" s="3"/>
       <c r="I111" s="3"/>
       <c r="J111" s="1">
@@ -5137,7 +5403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>217</v>
       </c>
@@ -5145,14 +5411,16 @@
         <v>218</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D112" s="3"/>
       <c r="E112" s="3"/>
       <c r="F112" s="3">
         <v>0</v>
       </c>
-      <c r="G112" s="3"/>
+      <c r="G112" s="3">
+        <v>0</v>
+      </c>
       <c r="H112" s="3"/>
       <c r="I112" s="3"/>
       <c r="J112" s="1">
@@ -5168,7 +5436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>219</v>
       </c>
@@ -5176,14 +5444,16 @@
         <v>220</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
       <c r="F113" s="3">
         <v>-653330657</v>
       </c>
-      <c r="G113" s="3"/>
+      <c r="G113" s="3">
+        <v>0</v>
+      </c>
       <c r="H113" s="3"/>
       <c r="I113" s="3"/>
       <c r="J113" s="1">
@@ -5199,7 +5469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>221</v>
       </c>
@@ -5207,14 +5477,16 @@
         <v>222</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
       <c r="F114" s="3">
         <v>341600000</v>
       </c>
-      <c r="G114" s="3"/>
+      <c r="G114" s="3">
+        <v>0</v>
+      </c>
       <c r="H114" s="3"/>
       <c r="I114" s="3"/>
       <c r="J114" s="1">
@@ -5230,7 +5502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>223</v>
       </c>
@@ -5238,14 +5510,16 @@
         <v>224</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D115" s="3"/>
       <c r="E115" s="3"/>
       <c r="F115" s="3">
         <v>537899388</v>
       </c>
-      <c r="G115" s="3"/>
+      <c r="G115" s="3">
+        <v>0</v>
+      </c>
       <c r="H115" s="3"/>
       <c r="I115" s="3"/>
       <c r="J115" s="1">
@@ -5261,7 +5535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>225</v>
       </c>
@@ -5269,14 +5543,16 @@
         <v>226</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
       <c r="F116" s="3">
         <v>7314355</v>
       </c>
-      <c r="G116" s="3"/>
+      <c r="G116" s="3">
+        <v>0</v>
+      </c>
       <c r="H116" s="3"/>
       <c r="I116" s="3"/>
       <c r="J116" s="1">
@@ -5292,7 +5568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>227</v>
       </c>
@@ -5300,14 +5576,16 @@
         <v>195</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D117" s="3"/>
       <c r="E117" s="3"/>
       <c r="F117" s="3">
         <v>0</v>
       </c>
-      <c r="G117" s="3"/>
+      <c r="G117" s="3">
+        <v>0</v>
+      </c>
       <c r="H117" s="3"/>
       <c r="I117" s="3"/>
       <c r="J117" s="1">
@@ -5323,7 +5601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>228</v>
       </c>
@@ -5331,14 +5609,16 @@
         <v>229</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D118" s="3"/>
       <c r="E118" s="3"/>
       <c r="F118" s="3">
         <v>4914996</v>
       </c>
-      <c r="G118" s="3"/>
+      <c r="G118" s="3">
+        <v>0</v>
+      </c>
       <c r="H118" s="3"/>
       <c r="I118" s="3"/>
       <c r="J118" s="1">
@@ -5354,7 +5634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>230</v>
       </c>
@@ -5362,14 +5642,16 @@
         <v>231</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D119" s="3"/>
       <c r="E119" s="3"/>
       <c r="F119" s="3">
         <v>3000000</v>
       </c>
-      <c r="G119" s="3"/>
+      <c r="G119" s="3">
+        <v>0</v>
+      </c>
       <c r="H119" s="3"/>
       <c r="I119" s="3"/>
       <c r="J119" s="1">
@@ -5385,7 +5667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>232</v>
       </c>
@@ -5393,14 +5675,16 @@
         <v>164</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
       <c r="F120" s="3">
         <v>0</v>
       </c>
-      <c r="G120" s="3"/>
+      <c r="G120" s="3">
+        <v>0</v>
+      </c>
       <c r="H120" s="3"/>
       <c r="I120" s="3"/>
       <c r="J120" s="1">
@@ -5416,7 +5700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>233</v>
       </c>
@@ -5424,14 +5708,16 @@
         <v>234</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D121" s="3"/>
       <c r="E121" s="3"/>
       <c r="F121" s="3">
         <v>80181681</v>
       </c>
-      <c r="G121" s="3"/>
+      <c r="G121" s="3">
+        <v>0</v>
+      </c>
       <c r="H121" s="3"/>
       <c r="I121" s="3"/>
       <c r="J121" s="1">
@@ -5447,7 +5733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>235</v>
       </c>
@@ -5455,14 +5741,16 @@
         <v>236</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D122" s="3"/>
       <c r="E122" s="3"/>
       <c r="F122" s="3">
         <v>227322131</v>
       </c>
-      <c r="G122" s="3"/>
+      <c r="G122" s="3">
+        <v>0</v>
+      </c>
       <c r="H122" s="3"/>
       <c r="I122" s="3"/>
       <c r="J122" s="1">
@@ -5478,7 +5766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>237</v>
       </c>
@@ -5486,14 +5774,16 @@
         <v>238</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D123" s="3"/>
       <c r="E123" s="3"/>
       <c r="F123" s="3">
         <v>595000</v>
       </c>
-      <c r="G123" s="3"/>
+      <c r="G123" s="3">
+        <v>0</v>
+      </c>
       <c r="H123" s="3"/>
       <c r="I123" s="3"/>
       <c r="J123" s="1">
@@ -5509,7 +5799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>239</v>
       </c>
@@ -5517,14 +5807,16 @@
         <v>240</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D124" s="3"/>
       <c r="E124" s="3"/>
       <c r="F124" s="3">
         <v>11775678</v>
       </c>
-      <c r="G124" s="3"/>
+      <c r="G124" s="3">
+        <v>0</v>
+      </c>
       <c r="H124" s="3"/>
       <c r="I124" s="3"/>
       <c r="J124" s="1">
@@ -5540,7 +5832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>241</v>
       </c>
@@ -5548,14 +5840,16 @@
         <v>242</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D125" s="3"/>
       <c r="E125" s="3"/>
       <c r="F125" s="3">
         <v>27120000</v>
       </c>
-      <c r="G125" s="3"/>
+      <c r="G125" s="3">
+        <v>0</v>
+      </c>
       <c r="H125" s="3"/>
       <c r="I125" s="3"/>
       <c r="J125" s="1">
@@ -5571,7 +5865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>243</v>
       </c>
@@ -5579,14 +5873,16 @@
         <v>244</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D126" s="3"/>
       <c r="E126" s="3"/>
       <c r="F126" s="3">
         <v>35469098</v>
       </c>
-      <c r="G126" s="3"/>
+      <c r="G126" s="3">
+        <v>0</v>
+      </c>
       <c r="H126" s="3"/>
       <c r="I126" s="3"/>
       <c r="J126" s="1">
@@ -5602,7 +5898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>245</v>
       </c>
@@ -5610,14 +5906,16 @@
         <v>246</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D127" s="3"/>
       <c r="E127" s="3"/>
       <c r="F127" s="3">
         <v>32922041</v>
       </c>
-      <c r="G127" s="3"/>
+      <c r="G127" s="3">
+        <v>0</v>
+      </c>
       <c r="H127" s="3"/>
       <c r="I127" s="3"/>
       <c r="J127" s="1">
@@ -5633,7 +5931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>247</v>
       </c>
@@ -5641,14 +5939,16 @@
         <v>248</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D128" s="3"/>
       <c r="E128" s="3"/>
       <c r="F128" s="3">
         <v>1462963</v>
       </c>
-      <c r="G128" s="3"/>
+      <c r="G128" s="3">
+        <v>0</v>
+      </c>
       <c r="H128" s="3"/>
       <c r="I128" s="3"/>
       <c r="J128" s="1">
@@ -5664,7 +5964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>249</v>
       </c>
@@ -5672,14 +5972,16 @@
         <v>166</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>
       <c r="F129" s="3">
         <v>38500248</v>
       </c>
-      <c r="G129" s="3"/>
+      <c r="G129" s="3">
+        <v>0</v>
+      </c>
       <c r="H129" s="3"/>
       <c r="I129" s="3"/>
       <c r="J129" s="1">
@@ -5695,7 +5997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>250</v>
       </c>
@@ -5703,11 +6005,13 @@
         <v>251</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D130" s="3"/>
       <c r="E130" s="3"/>
-      <c r="F130" s="3"/>
+      <c r="F130" s="3">
+        <v>0</v>
+      </c>
       <c r="G130" s="3">
         <v>4084968</v>
       </c>
@@ -5726,7 +6030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>252</v>
       </c>
@@ -5734,11 +6038,13 @@
         <v>253</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D131" s="3"/>
       <c r="E131" s="3"/>
-      <c r="F131" s="3"/>
+      <c r="F131" s="3">
+        <v>0</v>
+      </c>
       <c r="G131" s="3">
         <v>3560668</v>
       </c>
@@ -5757,7 +6063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>254</v>
       </c>
@@ -5765,11 +6071,13 @@
         <v>251</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D132" s="3"/>
       <c r="E132" s="3"/>
-      <c r="F132" s="3"/>
+      <c r="F132" s="3">
+        <v>0</v>
+      </c>
       <c r="G132" s="3">
         <v>524300</v>
       </c>
@@ -5788,7 +6096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>255</v>
       </c>
@@ -5796,14 +6104,16 @@
         <v>165</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D133" s="3"/>
       <c r="E133" s="3"/>
       <c r="F133" s="3">
         <v>76405356</v>
       </c>
-      <c r="G133" s="3"/>
+      <c r="G133" s="3">
+        <v>0</v>
+      </c>
       <c r="H133" s="3"/>
       <c r="I133" s="3"/>
       <c r="J133" s="1">
@@ -5819,7 +6129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>256</v>
       </c>
@@ -5827,14 +6137,16 @@
         <v>165</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D134" s="3"/>
       <c r="E134" s="3"/>
       <c r="F134" s="3">
         <v>76405356</v>
       </c>
-      <c r="G134" s="3"/>
+      <c r="G134" s="3">
+        <v>0</v>
+      </c>
       <c r="H134" s="3"/>
       <c r="I134" s="3"/>
       <c r="J134" s="1">
@@ -5850,7 +6162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>257</v>
       </c>
@@ -5858,14 +6170,16 @@
         <v>258</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D135" s="3"/>
       <c r="E135" s="3"/>
       <c r="F135" s="3">
         <v>123407221</v>
       </c>
-      <c r="G135" s="3"/>
+      <c r="G135" s="3">
+        <v>0</v>
+      </c>
       <c r="H135" s="3"/>
       <c r="I135" s="3"/>
       <c r="J135" s="1">
@@ -5881,7 +6195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>259</v>
       </c>
@@ -5889,14 +6203,16 @@
         <v>260</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="D136" s="3"/>
       <c r="E136" s="3"/>
       <c r="F136" s="3">
         <v>123407221</v>
       </c>
-      <c r="G136" s="3"/>
+      <c r="G136" s="3">
+        <v>0</v>
+      </c>
       <c r="H136" s="3"/>
       <c r="I136" s="3"/>
       <c r="J136" s="1">
@@ -5912,64 +6228,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="B137" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>276</v>
-      </c>
+    <row r="137" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D137" s="3"/>
       <c r="E137" s="3"/>
-      <c r="F137" s="3">
-        <v>9209788412</v>
-      </c>
-      <c r="G137" s="3">
-        <v>9209788412</v>
-      </c>
+      <c r="F137" s="3"/>
+      <c r="G137" s="3"/>
       <c r="H137" s="3"/>
       <c r="I137" s="3"/>
-      <c r="J137" s="1">
-        <v>1</v>
-      </c>
-      <c r="K137" s="1">
-        <v>1</v>
-      </c>
-      <c r="L137" s="1">
-        <v>1</v>
-      </c>
-      <c r="M137" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B138" s="4" t="s">
-        <v>263</v>
-      </c>
+    </row>
+    <row r="138" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B138" s="4"/>
       <c r="C138" s="4"/>
-      <c r="D138" s="5">
-        <v>14412370767</v>
-      </c>
-      <c r="E138" s="5">
-        <v>14412370767</v>
-      </c>
-      <c r="F138" s="5">
-        <v>74214664605</v>
-      </c>
-      <c r="G138" s="5">
-        <v>74214664605</v>
-      </c>
-      <c r="H138" s="5">
-        <v>14705622222</v>
-      </c>
-      <c r="I138" s="5">
-        <v>14705622222</v>
-      </c>
+      <c r="D138" s="5"/>
+      <c r="E138" s="5"/>
+      <c r="F138" s="5"/>
+      <c r="G138" s="5"/>
+      <c r="H138" s="5"/>
+      <c r="I138" s="5"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M136" xr:uid="{F67FFD85-9FD5-489C-9A0F-49D2F75178B7}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
Remove legacy mapping and artifact files
Deleted old financial statement mapping files, configuration files, and intermediate artifacts to clean up the repository. Added new VAS mapping registry and leadsheet revision documentation. Updated trial balance data files and notebook to reflect the new mapping approach based on TB-leaf prefix matching.
</commit_message>
<xml_diff>
--- a/data/TB_2024.xlsx
+++ b/data/TB_2024.xlsx
@@ -5,18 +5,18 @@
   <workbookPr saveExternalLinkValues="0" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/52ebbb93f357813a/10_Works/GitHub/Planning_Agent_NDD/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XA XUI - CVN\Documents\GitHub\Planning_Agent_NDD\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="13_ncr:1_{FA8BFFC3-FF41-44DA-A15C-5CC29DB30A53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F0D202B-8B78-442A-A14B-5AADD8BFAEC7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EA8657-EE38-424D-BA80-DD68E6532DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7784254E-2EFB-49AF-922A-1AA81A05D961}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7784254E-2EFB-49AF-922A-1AA81A05D961}"/>
   </bookViews>
   <sheets>
     <sheet name="GridViewExporter" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GridViewExporter!$A$1:$M$136</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">GridViewExporter!$A$1:$M$137</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="277">
   <si>
     <t>Số dư c.nợ</t>
   </si>
@@ -861,6 +861,12 @@
   </si>
   <si>
     <t>BS</t>
+  </si>
+  <si>
+    <t>33111x</t>
+  </si>
+  <si>
+    <t>Trả trước cho người bán</t>
   </si>
 </sst>
 </file>
@@ -878,15 +884,18 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1006,10 +1015,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1332,27 +1337,27 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:M138"/>
+  <dimension ref="A1:M139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C73" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomRight" activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="15.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="15.26953125" style="1" customWidth="1"/>
     <col min="10" max="11" width="7" style="1" customWidth="1"/>
-    <col min="12" max="12" width="5.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="8.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="5.81640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="8.1796875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="6" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>261</v>
       </c>
@@ -1393,7 +1398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1406,7 +1411,9 @@
       <c r="D2" s="3">
         <v>6605748426</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="3">
+        <v>0</v>
+      </c>
       <c r="F2" s="3">
         <v>11127312102</v>
       </c>
@@ -1432,7 +1439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1445,7 +1452,9 @@
       <c r="D3" s="3">
         <v>897868646</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="3">
+        <v>0</v>
+      </c>
       <c r="F3" s="3">
         <v>7698427237</v>
       </c>
@@ -1471,7 +1480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1484,7 +1493,9 @@
       <c r="D4" s="3">
         <v>897868646</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3">
+        <v>0</v>
+      </c>
       <c r="F4" s="3">
         <v>7698427237</v>
       </c>
@@ -1510,7 +1521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1523,7 +1534,9 @@
       <c r="D5" s="3">
         <v>5707879780</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="3">
+        <v>0</v>
+      </c>
       <c r="F5" s="3">
         <v>3428884865</v>
       </c>
@@ -1549,7 +1562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -1562,7 +1575,9 @@
       <c r="D6" s="3">
         <v>5707879780</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
       <c r="F6" s="3">
         <v>3428884865</v>
       </c>
@@ -1588,7 +1603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1598,8 +1613,12 @@
       <c r="C7" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
       <c r="F7" s="3">
         <v>834790638</v>
       </c>
@@ -1625,7 +1644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1635,8 +1654,12 @@
       <c r="C8" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
       <c r="F8" s="3">
         <v>834790638</v>
       </c>
@@ -1662,7 +1685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -1675,7 +1698,9 @@
       <c r="D9" s="3">
         <v>706266798</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
       <c r="F9" s="3">
         <v>8759317045</v>
       </c>
@@ -1701,7 +1726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -1714,7 +1739,9 @@
       <c r="D10" s="3">
         <v>706266798</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
       <c r="F10" s="3">
         <v>8759317045</v>
       </c>
@@ -1740,7 +1767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
@@ -1753,7 +1780,9 @@
       <c r="D11" s="3">
         <v>706266798</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
       <c r="F11" s="3">
         <v>8759317045</v>
       </c>
@@ -1779,7 +1808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -1792,7 +1821,9 @@
       <c r="D12" s="3">
         <v>124047295</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
       <c r="F12" s="3">
         <v>601203864</v>
       </c>
@@ -1818,7 +1849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -1831,7 +1862,9 @@
       <c r="D13" s="3">
         <v>124047295</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
       <c r="F13" s="3">
         <v>601203864</v>
       </c>
@@ -1857,7 +1890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1867,8 +1900,12 @@
       <c r="C14" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
       <c r="F14" s="3">
         <v>169643637</v>
       </c>
@@ -1894,7 +1931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1907,7 +1944,9 @@
       <c r="D15" s="3">
         <v>124047295</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
       <c r="F15" s="3">
         <v>431560227</v>
       </c>
@@ -1933,7 +1972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -1946,7 +1985,9 @@
       <c r="D16" s="3">
         <v>257292807</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="3">
+        <v>0</v>
+      </c>
       <c r="F16" s="3">
         <v>2773170553</v>
       </c>
@@ -1972,7 +2013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>31</v>
       </c>
@@ -1985,7 +2026,9 @@
       <c r="D17" s="3">
         <v>257292807</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
       <c r="F17" s="3">
         <v>2773170553</v>
       </c>
@@ -2011,7 +2054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -2024,7 +2067,9 @@
       <c r="D18" s="3">
         <v>257292807</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
       <c r="F18" s="3">
         <v>2773170553</v>
       </c>
@@ -2050,7 +2095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>34</v>
       </c>
@@ -2060,8 +2105,12 @@
       <c r="C19" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
       <c r="F19" s="3">
         <v>376652097</v>
       </c>
@@ -2087,7 +2136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>36</v>
       </c>
@@ -2100,7 +2149,9 @@
       <c r="D20" s="3">
         <v>257292807</v>
       </c>
-      <c r="E20" s="3"/>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
       <c r="F20" s="3">
         <v>2396518456</v>
       </c>
@@ -2126,7 +2177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>37</v>
       </c>
@@ -2139,7 +2190,9 @@
       <c r="D21" s="3">
         <v>123228000</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
       <c r="F21" s="3">
         <v>422174938</v>
       </c>
@@ -2165,7 +2218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>39</v>
       </c>
@@ -2175,8 +2228,12 @@
       <c r="C22" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
       <c r="F22" s="3">
         <v>590137877</v>
       </c>
@@ -2202,7 +2259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
@@ -2212,8 +2269,12 @@
       <c r="C23" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="D23" s="3">
+        <v>0</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
       <c r="F23" s="3">
         <v>590137877</v>
       </c>
@@ -2239,7 +2300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>43</v>
       </c>
@@ -2249,8 +2310,12 @@
       <c r="C24" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
       <c r="F24" s="3">
         <v>4762403069</v>
       </c>
@@ -2276,7 +2341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>45</v>
       </c>
@@ -2286,8 +2351,12 @@
       <c r="C25" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
       <c r="F25" s="3">
         <v>4762403069</v>
       </c>
@@ -2313,7 +2382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>47</v>
       </c>
@@ -2326,9 +2395,15 @@
       <c r="D26" s="3">
         <v>39320000</v>
       </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+      <c r="E26" s="3">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0</v>
+      </c>
       <c r="H26" s="3">
         <v>39320000</v>
       </c>
@@ -2348,7 +2423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>49</v>
       </c>
@@ -2361,9 +2436,15 @@
       <c r="D27" s="3">
         <v>39320000</v>
       </c>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+      <c r="E27" s="3">
+        <v>0</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0</v>
+      </c>
       <c r="H27" s="3">
         <v>39320000</v>
       </c>
@@ -2383,7 +2464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>51</v>
       </c>
@@ -2393,7 +2474,9 @@
       <c r="C28" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D28" s="3"/>
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
       <c r="E28" s="3">
         <v>18622374</v>
       </c>
@@ -2422,7 +2505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>53</v>
       </c>
@@ -2432,7 +2515,9 @@
       <c r="C29" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D29" s="3"/>
+      <c r="D29" s="3">
+        <v>0</v>
+      </c>
       <c r="E29" s="3">
         <v>18622374</v>
       </c>
@@ -2461,7 +2546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>55</v>
       </c>
@@ -2471,7 +2556,9 @@
       <c r="C30" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D30" s="3"/>
+      <c r="D30" s="3">
+        <v>0</v>
+      </c>
       <c r="E30" s="3">
         <v>18622374</v>
       </c>
@@ -2500,7 +2587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>57</v>
       </c>
@@ -2513,7 +2600,9 @@
       <c r="D31" s="3">
         <v>117685490</v>
       </c>
-      <c r="E31" s="3"/>
+      <c r="E31" s="3">
+        <v>0</v>
+      </c>
       <c r="F31" s="3">
         <v>1017423163</v>
       </c>
@@ -2539,7 +2628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>59</v>
       </c>
@@ -2552,7 +2641,9 @@
       <c r="D32" s="3">
         <v>101595093</v>
       </c>
-      <c r="E32" s="3"/>
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
       <c r="F32" s="3">
         <v>978349526</v>
       </c>
@@ -2578,7 +2669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>61</v>
       </c>
@@ -2588,8 +2679,12 @@
       <c r="C33" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
+      <c r="D33" s="3">
+        <v>0</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0</v>
+      </c>
       <c r="F33" s="3">
         <v>10890000</v>
       </c>
@@ -2615,7 +2710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>63</v>
       </c>
@@ -2628,7 +2723,9 @@
       <c r="D34" s="3">
         <v>101595093</v>
       </c>
-      <c r="E34" s="3"/>
+      <c r="E34" s="3">
+        <v>0</v>
+      </c>
       <c r="F34" s="3">
         <v>967459526</v>
       </c>
@@ -2654,7 +2751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>65</v>
       </c>
@@ -2667,7 +2764,9 @@
       <c r="D35" s="3">
         <v>16090397</v>
       </c>
-      <c r="E35" s="3"/>
+      <c r="E35" s="3">
+        <v>0</v>
+      </c>
       <c r="F35" s="3">
         <v>39073637</v>
       </c>
@@ -2693,7 +2792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>67</v>
       </c>
@@ -2706,7 +2805,9 @@
       <c r="D36" s="3">
         <v>10549745</v>
       </c>
-      <c r="E36" s="3"/>
+      <c r="E36" s="3">
+        <v>0</v>
+      </c>
       <c r="F36" s="3">
         <v>30950000</v>
       </c>
@@ -2732,7 +2833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>69</v>
       </c>
@@ -2745,7 +2846,9 @@
       <c r="D37" s="3">
         <v>5540652</v>
       </c>
-      <c r="E37" s="3"/>
+      <c r="E37" s="3">
+        <v>0</v>
+      </c>
       <c r="F37" s="3">
         <v>8123637</v>
       </c>
@@ -2771,7 +2874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>71</v>
       </c>
@@ -2784,9 +2887,15 @@
       <c r="D38" s="3">
         <v>148099200</v>
       </c>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
+      <c r="E38" s="3">
+        <v>0</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0</v>
+      </c>
+      <c r="G38" s="3">
+        <v>0</v>
+      </c>
       <c r="H38" s="3">
         <v>148099200</v>
       </c>
@@ -2806,7 +2915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>73</v>
       </c>
@@ -2819,9 +2928,15 @@
       <c r="D39" s="3">
         <v>148099200</v>
       </c>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
+      <c r="E39" s="3">
+        <v>0</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0</v>
+      </c>
+      <c r="G39" s="3">
+        <v>0</v>
+      </c>
       <c r="H39" s="3">
         <v>148099200</v>
       </c>
@@ -2841,7 +2956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>75</v>
       </c>
@@ -2882,7 +2997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>77</v>
       </c>
@@ -2923,7 +3038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>79</v>
       </c>
@@ -2946,7 +3061,7 @@
         <v>2643586171</v>
       </c>
       <c r="H42" s="3">
-        <v>19175523</v>
+        <v>0</v>
       </c>
       <c r="I42" s="3">
         <v>73248899</v>
@@ -2964,31 +3079,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>81</v>
+        <v>275</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>82</v>
+        <v>276</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D43" s="3"/>
+      <c r="D43" s="3">
+        <v>0</v>
+      </c>
       <c r="E43" s="3">
-        <v>123278400</v>
+        <v>0</v>
       </c>
       <c r="F43" s="3">
-        <v>4193742227</v>
+        <v>0</v>
       </c>
       <c r="G43" s="3">
-        <v>4393777280</v>
+        <v>0</v>
       </c>
       <c r="H43" s="3">
-        <v>0</v>
+        <v>19175523</v>
       </c>
       <c r="I43" s="3">
-        <v>323313453</v>
+        <v>0</v>
       </c>
       <c r="J43" s="1">
         <v>0</v>
@@ -3003,99 +3120,109 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0</v>
+      </c>
+      <c r="E44" s="3">
+        <v>123278400</v>
+      </c>
+      <c r="F44" s="3">
+        <v>4193742227</v>
+      </c>
+      <c r="G44" s="3">
+        <v>4393777280</v>
+      </c>
+      <c r="H44" s="3">
+        <v>0</v>
+      </c>
+      <c r="I44" s="3">
+        <v>323313453</v>
+      </c>
+      <c r="J44" s="1">
+        <v>0</v>
+      </c>
+      <c r="K44" s="1">
+        <v>1</v>
+      </c>
+      <c r="L44" s="1">
+        <v>3</v>
+      </c>
+      <c r="M44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3">
+      <c r="C45" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D45" s="3">
+        <v>0</v>
+      </c>
+      <c r="E45" s="3">
         <v>129447947</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F45" s="3">
         <v>2439216613</v>
       </c>
-      <c r="G44" s="3">
+      <c r="G45" s="3">
         <v>2330478004</v>
       </c>
-      <c r="H44" s="3">
-        <v>0</v>
-      </c>
-      <c r="I44" s="3">
+      <c r="H45" s="3">
+        <v>0</v>
+      </c>
+      <c r="I45" s="3">
         <v>20709338</v>
       </c>
-      <c r="J44" s="1">
-        <v>1</v>
-      </c>
-      <c r="K44" s="1">
-        <v>0</v>
-      </c>
-      <c r="L44" s="1">
-        <v>1</v>
-      </c>
-      <c r="M44" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="1" t="s">
+      <c r="J45" s="1">
+        <v>1</v>
+      </c>
+      <c r="K45" s="1">
+        <v>0</v>
+      </c>
+      <c r="L45" s="1">
+        <v>1</v>
+      </c>
+      <c r="M45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3">
+      <c r="C46" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D46" s="3">
+        <v>0</v>
+      </c>
+      <c r="E46" s="3">
+        <v>0</v>
+      </c>
+      <c r="F46" s="3">
         <v>1072629402</v>
       </c>
-      <c r="G45" s="3">
+      <c r="G46" s="3">
         <v>1089985368</v>
-      </c>
-      <c r="H45" s="3">
-        <v>0</v>
-      </c>
-      <c r="I45" s="3">
-        <v>17355966</v>
-      </c>
-      <c r="J45" s="1">
-        <v>0</v>
-      </c>
-      <c r="K45" s="1">
-        <v>0</v>
-      </c>
-      <c r="L45" s="1">
-        <v>2</v>
-      </c>
-      <c r="M45" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3">
-        <v>725251159</v>
-      </c>
-      <c r="G46" s="3">
-        <v>742607125</v>
       </c>
       <c r="H46" s="3">
         <v>0</v>
@@ -3110,24 +3237,28 @@
         <v>0</v>
       </c>
       <c r="L46" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M46" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
+      <c r="D47" s="3">
+        <v>0</v>
+      </c>
+      <c r="E47" s="3">
+        <v>0</v>
+      </c>
       <c r="F47" s="3">
         <v>725251159</v>
       </c>
@@ -3144,143 +3275,159 @@
         <v>0</v>
       </c>
       <c r="K47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L47" s="1">
+        <v>3</v>
+      </c>
+      <c r="M47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D48" s="3">
+        <v>0</v>
+      </c>
+      <c r="E48" s="3">
+        <v>0</v>
+      </c>
+      <c r="F48" s="3">
+        <v>725251159</v>
+      </c>
+      <c r="G48" s="3">
+        <v>742607125</v>
+      </c>
+      <c r="H48" s="3">
+        <v>0</v>
+      </c>
+      <c r="I48" s="3">
+        <v>17355966</v>
+      </c>
+      <c r="J48" s="1">
+        <v>0</v>
+      </c>
+      <c r="K48" s="1">
+        <v>1</v>
+      </c>
+      <c r="L48" s="1">
         <v>4</v>
       </c>
-      <c r="M47" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+      <c r="M48" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3">
+      <c r="C49" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D49" s="3">
+        <v>0</v>
+      </c>
+      <c r="E49" s="3">
+        <v>0</v>
+      </c>
+      <c r="F49" s="3">
         <v>347378243</v>
       </c>
-      <c r="G48" s="3">
+      <c r="G49" s="3">
         <v>347378243</v>
       </c>
-      <c r="H48" s="3">
-        <v>0</v>
-      </c>
-      <c r="I48" s="3">
-        <v>0</v>
-      </c>
-      <c r="J48" s="1">
-        <v>0</v>
-      </c>
-      <c r="K48" s="1">
-        <v>1</v>
-      </c>
-      <c r="L48" s="1">
+      <c r="H49" s="3">
+        <v>0</v>
+      </c>
+      <c r="I49" s="3">
+        <v>0</v>
+      </c>
+      <c r="J49" s="1">
+        <v>0</v>
+      </c>
+      <c r="K49" s="1">
+        <v>1</v>
+      </c>
+      <c r="L49" s="1">
         <v>3</v>
       </c>
-      <c r="M48" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
+      <c r="M49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3">
+      <c r="C50" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D50" s="3">
+        <v>0</v>
+      </c>
+      <c r="E50" s="3">
+        <v>0</v>
+      </c>
+      <c r="F50" s="3">
         <v>10640416</v>
       </c>
-      <c r="G49" s="3">
+      <c r="G50" s="3">
         <v>10640416</v>
       </c>
-      <c r="H49" s="3">
-        <v>0</v>
-      </c>
-      <c r="I49" s="3">
-        <v>0</v>
-      </c>
-      <c r="J49" s="1">
-        <v>0</v>
-      </c>
-      <c r="K49" s="1">
-        <v>0</v>
-      </c>
-      <c r="L49" s="1">
+      <c r="H50" s="3">
+        <v>0</v>
+      </c>
+      <c r="I50" s="3">
+        <v>0</v>
+      </c>
+      <c r="J50" s="1">
+        <v>0</v>
+      </c>
+      <c r="K50" s="1">
+        <v>0</v>
+      </c>
+      <c r="L50" s="1">
         <v>2</v>
       </c>
-      <c r="M49" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
+      <c r="M50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3">
+      <c r="C51" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D51" s="3">
+        <v>0</v>
+      </c>
+      <c r="E51" s="3">
+        <v>0</v>
+      </c>
+      <c r="F51" s="3">
         <v>5295224</v>
       </c>
-      <c r="G50" s="3">
+      <c r="G51" s="3">
         <v>5295224</v>
-      </c>
-      <c r="H50" s="3">
-        <v>0</v>
-      </c>
-      <c r="I50" s="3">
-        <v>0</v>
-      </c>
-      <c r="J50" s="1">
-        <v>0</v>
-      </c>
-      <c r="K50" s="1">
-        <v>1</v>
-      </c>
-      <c r="L50" s="1">
-        <v>3</v>
-      </c>
-      <c r="M50" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3">
-        <v>5345192</v>
-      </c>
-      <c r="G51" s="3">
-        <v>5345192</v>
       </c>
       <c r="H51" s="3">
         <v>0</v>
@@ -3301,68 +3448,74 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D52" s="3">
+        <v>0</v>
+      </c>
+      <c r="E52" s="3">
+        <v>0</v>
+      </c>
+      <c r="F52" s="3">
+        <v>5345192</v>
+      </c>
+      <c r="G52" s="3">
+        <v>5345192</v>
+      </c>
+      <c r="H52" s="3">
+        <v>0</v>
+      </c>
+      <c r="I52" s="3">
+        <v>0</v>
+      </c>
+      <c r="J52" s="1">
+        <v>0</v>
+      </c>
+      <c r="K52" s="1">
+        <v>1</v>
+      </c>
+      <c r="L52" s="1">
+        <v>3</v>
+      </c>
+      <c r="M52" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B53" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3">
+      <c r="C53" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D53" s="3">
+        <v>0</v>
+      </c>
+      <c r="E53" s="3">
+        <v>0</v>
+      </c>
+      <c r="F53" s="3">
         <v>123407221</v>
       </c>
-      <c r="G52" s="3">
+      <c r="G53" s="3">
         <v>123407221</v>
       </c>
-      <c r="H52" s="3">
-        <v>0</v>
-      </c>
-      <c r="I52" s="3">
-        <v>0</v>
-      </c>
-      <c r="J52" s="1">
-        <v>0</v>
-      </c>
-      <c r="K52" s="1">
-        <v>1</v>
-      </c>
-      <c r="L52" s="1">
-        <v>2</v>
-      </c>
-      <c r="M52" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3">
-        <v>129447947</v>
-      </c>
-      <c r="F53" s="3">
-        <v>1219413632</v>
-      </c>
-      <c r="G53" s="3">
-        <v>1093319057</v>
-      </c>
       <c r="H53" s="3">
         <v>0</v>
       </c>
       <c r="I53" s="3">
-        <v>3353372</v>
+        <v>0</v>
       </c>
       <c r="J53" s="1">
         <v>0</v>
@@ -3377,35 +3530,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
+      <c r="D54" s="3">
+        <v>0</v>
+      </c>
+      <c r="E54" s="3">
+        <v>129447947</v>
+      </c>
       <c r="F54" s="3">
-        <v>9485942</v>
+        <v>1219413632</v>
       </c>
       <c r="G54" s="3">
-        <v>9485942</v>
+        <v>1093319057</v>
       </c>
       <c r="H54" s="3">
         <v>0</v>
       </c>
       <c r="I54" s="3">
-        <v>0</v>
+        <v>3353372</v>
       </c>
       <c r="J54" s="1">
         <v>0</v>
       </c>
       <c r="K54" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L54" s="1">
         <v>2</v>
@@ -3414,18 +3571,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
+      <c r="D55" s="3">
+        <v>0</v>
+      </c>
+      <c r="E55" s="3">
+        <v>0</v>
+      </c>
       <c r="F55" s="3">
         <v>9485942</v>
       </c>
@@ -3442,64 +3603,72 @@
         <v>0</v>
       </c>
       <c r="K55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L55" s="1">
+        <v>2</v>
+      </c>
+      <c r="M55" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D56" s="3">
+        <v>0</v>
+      </c>
+      <c r="E56" s="3">
+        <v>0</v>
+      </c>
+      <c r="F56" s="3">
+        <v>9485942</v>
+      </c>
+      <c r="G56" s="3">
+        <v>9485942</v>
+      </c>
+      <c r="H56" s="3">
+        <v>0</v>
+      </c>
+      <c r="I56" s="3">
+        <v>0</v>
+      </c>
+      <c r="J56" s="1">
+        <v>0</v>
+      </c>
+      <c r="K56" s="1">
+        <v>1</v>
+      </c>
+      <c r="L56" s="1">
         <v>3</v>
       </c>
-      <c r="M55" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="1" t="s">
+      <c r="M56" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B57" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3">
-        <v>3640000</v>
-      </c>
-      <c r="G56" s="3">
-        <v>3640000</v>
-      </c>
-      <c r="H56" s="3">
-        <v>0</v>
-      </c>
-      <c r="I56" s="3">
-        <v>0</v>
-      </c>
-      <c r="J56" s="1">
-        <v>0</v>
-      </c>
-      <c r="K56" s="1">
-        <v>0</v>
-      </c>
-      <c r="L56" s="1">
-        <v>2</v>
-      </c>
-      <c r="M56" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="C57" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
+      <c r="D57" s="3">
+        <v>0</v>
+      </c>
+      <c r="E57" s="3">
+        <v>0</v>
+      </c>
       <c r="F57" s="3">
         <v>3640000</v>
       </c>
@@ -3516,57 +3685,59 @@
         <v>0</v>
       </c>
       <c r="K57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L57" s="1">
+        <v>2</v>
+      </c>
+      <c r="M57" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D58" s="3">
+        <v>0</v>
+      </c>
+      <c r="E58" s="3">
+        <v>0</v>
+      </c>
+      <c r="F58" s="3">
+        <v>3640000</v>
+      </c>
+      <c r="G58" s="3">
+        <v>3640000</v>
+      </c>
+      <c r="H58" s="3">
+        <v>0</v>
+      </c>
+      <c r="I58" s="3">
+        <v>0</v>
+      </c>
+      <c r="J58" s="1">
+        <v>0</v>
+      </c>
+      <c r="K58" s="1">
+        <v>1</v>
+      </c>
+      <c r="L58" s="1">
         <v>3</v>
       </c>
-      <c r="M57" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="1" t="s">
+      <c r="M58" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3">
-        <v>24422231</v>
-      </c>
-      <c r="F58" s="3">
-        <v>1516294162</v>
-      </c>
-      <c r="G58" s="3">
-        <v>1540017016</v>
-      </c>
-      <c r="H58" s="3">
-        <v>0</v>
-      </c>
-      <c r="I58" s="3">
-        <v>48145085</v>
-      </c>
-      <c r="J58" s="1">
-        <v>1</v>
-      </c>
-      <c r="K58" s="1">
-        <v>0</v>
-      </c>
-      <c r="L58" s="1">
-        <v>1</v>
-      </c>
-      <c r="M58" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>112</v>
@@ -3574,7 +3745,9 @@
       <c r="C59" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D59" s="3"/>
+      <c r="D59" s="3">
+        <v>0</v>
+      </c>
       <c r="E59" s="3">
         <v>24422231</v>
       </c>
@@ -3591,37 +3764,39 @@
         <v>48145085</v>
       </c>
       <c r="J59" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K59" s="1">
         <v>0</v>
       </c>
       <c r="L59" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M59" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D60" s="3"/>
+      <c r="D60" s="3">
+        <v>0</v>
+      </c>
       <c r="E60" s="3">
         <v>24422231</v>
       </c>
       <c r="F60" s="3">
-        <v>543926968</v>
+        <v>1516294162</v>
       </c>
       <c r="G60" s="3">
-        <v>567649822</v>
+        <v>1540017016</v>
       </c>
       <c r="H60" s="3">
         <v>0</v>
@@ -3633,38 +3808,42 @@
         <v>0</v>
       </c>
       <c r="K60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L60" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M60" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
+      <c r="D61" s="3">
+        <v>0</v>
+      </c>
+      <c r="E61" s="3">
+        <v>24422231</v>
+      </c>
       <c r="F61" s="3">
-        <v>972367194</v>
+        <v>543926968</v>
       </c>
       <c r="G61" s="3">
-        <v>972367194</v>
+        <v>567649822</v>
       </c>
       <c r="H61" s="3">
         <v>0</v>
       </c>
       <c r="I61" s="3">
-        <v>0</v>
+        <v>48145085</v>
       </c>
       <c r="J61" s="1">
         <v>0</v>
@@ -3679,138 +3858,150 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D62" s="3">
+        <v>0</v>
+      </c>
+      <c r="E62" s="3">
+        <v>0</v>
+      </c>
+      <c r="F62" s="3">
+        <v>972367194</v>
+      </c>
+      <c r="G62" s="3">
+        <v>972367194</v>
+      </c>
+      <c r="H62" s="3">
+        <v>0</v>
+      </c>
+      <c r="I62" s="3">
+        <v>0</v>
+      </c>
+      <c r="J62" s="1">
+        <v>0</v>
+      </c>
+      <c r="K62" s="1">
+        <v>1</v>
+      </c>
+      <c r="L62" s="1">
+        <v>3</v>
+      </c>
+      <c r="M62" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="B63" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3">
+      <c r="C63" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D63" s="3">
+        <v>0</v>
+      </c>
+      <c r="E63" s="3">
         <v>309852397</v>
       </c>
-      <c r="F62" s="3">
+      <c r="F63" s="3">
         <v>103372000</v>
       </c>
-      <c r="G62" s="3">
+      <c r="G63" s="3">
         <v>212615391</v>
       </c>
-      <c r="H62" s="3">
-        <v>0</v>
-      </c>
-      <c r="I62" s="3">
+      <c r="H63" s="3">
+        <v>0</v>
+      </c>
+      <c r="I63" s="3">
         <v>419095788</v>
       </c>
-      <c r="J62" s="1">
-        <v>1</v>
-      </c>
-      <c r="K62" s="1">
-        <v>1</v>
-      </c>
-      <c r="L62" s="1">
-        <v>1</v>
-      </c>
-      <c r="M62" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="1" t="s">
+      <c r="J63" s="1">
+        <v>1</v>
+      </c>
+      <c r="K63" s="1">
+        <v>1</v>
+      </c>
+      <c r="L63" s="1">
+        <v>1</v>
+      </c>
+      <c r="M63" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B64" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3">
+      <c r="C64" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D64" s="3">
+        <v>0</v>
+      </c>
+      <c r="E64" s="3">
         <v>25111318</v>
       </c>
-      <c r="F63" s="3">
+      <c r="F64" s="3">
         <v>1048632661</v>
       </c>
-      <c r="G63" s="3">
+      <c r="G64" s="3">
         <v>1070178636</v>
       </c>
-      <c r="H63" s="3">
-        <v>0</v>
-      </c>
-      <c r="I63" s="3">
+      <c r="H64" s="3">
+        <v>0</v>
+      </c>
+      <c r="I64" s="3">
         <v>46657293</v>
       </c>
-      <c r="J63" s="1">
-        <v>1</v>
-      </c>
-      <c r="K63" s="1">
-        <v>0</v>
-      </c>
-      <c r="L63" s="1">
-        <v>1</v>
-      </c>
-      <c r="M63" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="1" t="s">
+      <c r="J64" s="1">
+        <v>1</v>
+      </c>
+      <c r="K64" s="1">
+        <v>0</v>
+      </c>
+      <c r="L64" s="1">
+        <v>1</v>
+      </c>
+      <c r="M64" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B65" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3">
+      <c r="C65" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D65" s="3">
+        <v>0</v>
+      </c>
+      <c r="E65" s="3">
+        <v>0</v>
+      </c>
+      <c r="F65" s="3">
         <v>9302858</v>
       </c>
-      <c r="G64" s="3">
+      <c r="G65" s="3">
         <v>9302858</v>
-      </c>
-      <c r="H64" s="3">
-        <v>0</v>
-      </c>
-      <c r="I64" s="3">
-        <v>0</v>
-      </c>
-      <c r="J64" s="1">
-        <v>0</v>
-      </c>
-      <c r="K64" s="1">
-        <v>1</v>
-      </c>
-      <c r="L64" s="1">
-        <v>2</v>
-      </c>
-      <c r="M64" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3">
-        <v>118611455</v>
-      </c>
-      <c r="G65" s="3">
-        <v>118611455</v>
       </c>
       <c r="H65" s="3">
         <v>0</v>
@@ -3831,23 +4022,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
+      <c r="D66" s="3">
+        <v>0</v>
+      </c>
+      <c r="E66" s="3">
+        <v>0</v>
+      </c>
       <c r="F66" s="3">
-        <v>20931432</v>
+        <v>118611455</v>
       </c>
       <c r="G66" s="3">
-        <v>20931432</v>
+        <v>118611455</v>
       </c>
       <c r="H66" s="3">
         <v>0</v>
@@ -3868,23 +4063,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
+      <c r="D67" s="3">
+        <v>0</v>
+      </c>
+      <c r="E67" s="3">
+        <v>0</v>
+      </c>
       <c r="F67" s="3">
-        <v>9302864</v>
+        <v>20931432</v>
       </c>
       <c r="G67" s="3">
-        <v>9302864</v>
+        <v>20931432</v>
       </c>
       <c r="H67" s="3">
         <v>0</v>
@@ -3905,56 +4104,60 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D68" s="3"/>
+      <c r="D68" s="3">
+        <v>0</v>
+      </c>
       <c r="E68" s="3">
-        <v>25111318</v>
+        <v>0</v>
       </c>
       <c r="F68" s="3">
-        <v>890484052</v>
+        <v>9302864</v>
       </c>
       <c r="G68" s="3">
-        <v>912030027</v>
+        <v>9302864</v>
       </c>
       <c r="H68" s="3">
         <v>0</v>
       </c>
       <c r="I68" s="3">
-        <v>46657293</v>
+        <v>0</v>
       </c>
       <c r="J68" s="1">
         <v>0</v>
       </c>
       <c r="K68" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L68" s="1">
         <v>2</v>
       </c>
       <c r="M68" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D69" s="3"/>
+      <c r="D69" s="3">
+        <v>0</v>
+      </c>
       <c r="E69" s="3">
         <v>25111318</v>
       </c>
@@ -3977,15 +4180,15 @@
         <v>0</v>
       </c>
       <c r="L69" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M69" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>132</v>
@@ -3993,7 +4196,9 @@
       <c r="C70" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D70" s="3"/>
+      <c r="D70" s="3">
+        <v>0</v>
+      </c>
       <c r="E70" s="3">
         <v>25111318</v>
       </c>
@@ -4013,66 +4218,78 @@
         <v>0</v>
       </c>
       <c r="K70" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L70" s="1">
+        <v>3</v>
+      </c>
+      <c r="M70" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D71" s="3">
+        <v>0</v>
+      </c>
+      <c r="E71" s="3">
+        <v>25111318</v>
+      </c>
+      <c r="F71" s="3">
+        <v>890484052</v>
+      </c>
+      <c r="G71" s="3">
+        <v>912030027</v>
+      </c>
+      <c r="H71" s="3">
+        <v>0</v>
+      </c>
+      <c r="I71" s="3">
+        <v>46657293</v>
+      </c>
+      <c r="J71" s="1">
+        <v>0</v>
+      </c>
+      <c r="K71" s="1">
+        <v>1</v>
+      </c>
+      <c r="L71" s="1">
         <v>4</v>
       </c>
-      <c r="M70" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="1" t="s">
+      <c r="M71" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B72" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D71" s="3"/>
-      <c r="E71" s="3">
-        <v>13746000000</v>
-      </c>
-      <c r="F71" s="3"/>
-      <c r="G71" s="3"/>
-      <c r="H71" s="3">
-        <v>0</v>
-      </c>
-      <c r="I71" s="3">
-        <v>13746000000</v>
-      </c>
-      <c r="J71" s="1">
-        <v>1</v>
-      </c>
-      <c r="K71" s="1">
-        <v>0</v>
-      </c>
-      <c r="L71" s="1">
-        <v>1</v>
-      </c>
-      <c r="M71" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="C72" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D72" s="3"/>
+      <c r="D72" s="3">
+        <v>0</v>
+      </c>
       <c r="E72" s="3">
         <v>13746000000</v>
       </c>
-      <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
+      <c r="F72" s="3">
+        <v>0</v>
+      </c>
+      <c r="G72" s="3">
+        <v>0</v>
+      </c>
       <c r="H72" s="3">
         <v>0</v>
       </c>
@@ -4080,67 +4297,75 @@
         <v>13746000000</v>
       </c>
       <c r="J72" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K72" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L72" s="1">
+        <v>1</v>
+      </c>
+      <c r="M72" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D73" s="3">
+        <v>0</v>
+      </c>
+      <c r="E73" s="3">
+        <v>13746000000</v>
+      </c>
+      <c r="F73" s="3">
+        <v>0</v>
+      </c>
+      <c r="G73" s="3">
+        <v>0</v>
+      </c>
+      <c r="H73" s="3">
+        <v>0</v>
+      </c>
+      <c r="I73" s="3">
+        <v>13746000000</v>
+      </c>
+      <c r="J73" s="1">
+        <v>0</v>
+      </c>
+      <c r="K73" s="1">
+        <v>1</v>
+      </c>
+      <c r="L73" s="1">
         <v>2</v>
       </c>
-      <c r="M72" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="1" t="s">
+      <c r="M73" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D73" s="3"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3">
-        <v>76685</v>
-      </c>
-      <c r="G73" s="3">
-        <v>76685</v>
-      </c>
-      <c r="H73" s="3">
-        <v>0</v>
-      </c>
-      <c r="I73" s="3">
-        <v>0</v>
-      </c>
-      <c r="J73" s="1">
-        <v>1</v>
-      </c>
-      <c r="K73" s="1">
-        <v>0</v>
-      </c>
-      <c r="L73" s="1">
-        <v>1</v>
-      </c>
-      <c r="M73" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="C74" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
+      <c r="D74" s="3">
+        <v>0</v>
+      </c>
+      <c r="E74" s="3">
+        <v>0</v>
+      </c>
       <c r="F74" s="3">
         <v>76685</v>
       </c>
@@ -4154,116 +4379,124 @@
         <v>0</v>
       </c>
       <c r="J74" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K74" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L74" s="1">
+        <v>1</v>
+      </c>
+      <c r="M74" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D75" s="3">
+        <v>0</v>
+      </c>
+      <c r="E75" s="3">
+        <v>0</v>
+      </c>
+      <c r="F75" s="3">
+        <v>76685</v>
+      </c>
+      <c r="G75" s="3">
+        <v>76685</v>
+      </c>
+      <c r="H75" s="3">
+        <v>0</v>
+      </c>
+      <c r="I75" s="3">
+        <v>0</v>
+      </c>
+      <c r="J75" s="1">
+        <v>0</v>
+      </c>
+      <c r="K75" s="1">
+        <v>1</v>
+      </c>
+      <c r="L75" s="1">
         <v>2</v>
       </c>
-      <c r="M74" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
+      <c r="M75" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B76" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D75" s="3">
+      <c r="C76" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D76" s="3">
         <v>6290591391</v>
       </c>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3">
+      <c r="E76" s="3">
+        <v>0</v>
+      </c>
+      <c r="F76" s="3">
         <v>3392674899</v>
       </c>
-      <c r="G75" s="3">
+      <c r="G76" s="3">
         <v>3383468524</v>
       </c>
-      <c r="H75" s="3">
+      <c r="H76" s="3">
         <v>6299797766</v>
       </c>
-      <c r="I75" s="3">
-        <v>0</v>
-      </c>
-      <c r="J75" s="1">
-        <v>1</v>
-      </c>
-      <c r="K75" s="1">
-        <v>0</v>
-      </c>
-      <c r="L75" s="1">
-        <v>1</v>
-      </c>
-      <c r="M75" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
+      <c r="I76" s="3">
+        <v>0</v>
+      </c>
+      <c r="J76" s="1">
+        <v>1</v>
+      </c>
+      <c r="K76" s="1">
+        <v>0</v>
+      </c>
+      <c r="L76" s="1">
+        <v>1</v>
+      </c>
+      <c r="M76" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B77" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D76" s="3">
+      <c r="C77" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D77" s="3">
         <v>4171107126</v>
       </c>
-      <c r="E76" s="3"/>
-      <c r="F76" s="3">
+      <c r="E77" s="3">
+        <v>0</v>
+      </c>
+      <c r="F77" s="3">
         <v>2119484265</v>
       </c>
-      <c r="G76" s="3"/>
-      <c r="H76" s="3">
+      <c r="G77" s="3">
+        <v>0</v>
+      </c>
+      <c r="H77" s="3">
         <v>6290591391</v>
-      </c>
-      <c r="I76" s="3">
-        <v>0</v>
-      </c>
-      <c r="J76" s="1">
-        <v>0</v>
-      </c>
-      <c r="K76" s="1">
-        <v>1</v>
-      </c>
-      <c r="L76" s="1">
-        <v>2</v>
-      </c>
-      <c r="M76" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D77" s="3">
-        <v>2119484265</v>
-      </c>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3">
-        <v>1273190634</v>
-      </c>
-      <c r="G77" s="3">
-        <v>3383468524</v>
-      </c>
-      <c r="H77" s="3">
-        <v>9206375</v>
       </c>
       <c r="I77" s="3">
         <v>0</v>
@@ -4281,45 +4514,53 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="D78" s="3">
+        <v>2119484265</v>
+      </c>
+      <c r="E78" s="3">
+        <v>0</v>
+      </c>
+      <c r="F78" s="3">
+        <v>1273190634</v>
+      </c>
+      <c r="G78" s="3">
+        <v>3383468524</v>
+      </c>
+      <c r="H78" s="3">
+        <v>9206375</v>
+      </c>
+      <c r="I78" s="3">
+        <v>0</v>
+      </c>
+      <c r="J78" s="1">
+        <v>0</v>
+      </c>
+      <c r="K78" s="1">
+        <v>1</v>
+      </c>
+      <c r="L78" s="1">
+        <v>2</v>
+      </c>
+      <c r="M78" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B79" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D78" s="3"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3">
-        <v>0</v>
-      </c>
-      <c r="G78" s="3">
-        <v>0</v>
-      </c>
-      <c r="H78" s="3"/>
-      <c r="I78" s="3"/>
-      <c r="J78" s="1">
-        <v>1</v>
-      </c>
-      <c r="K78" s="1">
-        <v>0</v>
-      </c>
-      <c r="L78" s="1">
-        <v>1</v>
-      </c>
-      <c r="M78" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>273</v>
@@ -4330,29 +4571,29 @@
         <v>0</v>
       </c>
       <c r="G79" s="3">
-        <v>6421735813</v>
+        <v>0</v>
       </c>
       <c r="H79" s="3"/>
       <c r="I79" s="3"/>
       <c r="J79" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K79" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L79" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M79" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>273</v>
@@ -4363,7 +4604,7 @@
         <v>0</v>
       </c>
       <c r="G80" s="3">
-        <v>596942428</v>
+        <v>6421735813</v>
       </c>
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
@@ -4380,12 +4621,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>273</v>
@@ -4396,7 +4637,7 @@
         <v>0</v>
       </c>
       <c r="G81" s="3">
-        <v>784740170</v>
+        <v>596942428</v>
       </c>
       <c r="H81" s="3"/>
       <c r="I81" s="3"/>
@@ -4413,12 +4654,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>273</v>
@@ -4429,29 +4670,29 @@
         <v>0</v>
       </c>
       <c r="G82" s="3">
-        <v>0</v>
+        <v>784740170</v>
       </c>
       <c r="H82" s="3"/>
       <c r="I82" s="3"/>
       <c r="J82" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K82" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L82" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M82" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>273</v>
@@ -4462,29 +4703,29 @@
         <v>0</v>
       </c>
       <c r="G83" s="3">
-        <v>997616</v>
+        <v>0</v>
       </c>
       <c r="H83" s="3"/>
       <c r="I83" s="3"/>
       <c r="J83" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L83" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M83" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>273</v>
@@ -4495,7 +4736,7 @@
         <v>0</v>
       </c>
       <c r="G84" s="3">
-        <v>154099165</v>
+        <v>997616</v>
       </c>
       <c r="H84" s="3"/>
       <c r="I84" s="3"/>
@@ -4512,12 +4753,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>273</v>
@@ -4528,7 +4769,7 @@
         <v>0</v>
       </c>
       <c r="G85" s="3">
-        <v>-26002382</v>
+        <v>154099165</v>
       </c>
       <c r="H85" s="3"/>
       <c r="I85" s="3"/>
@@ -4545,12 +4786,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>273</v>
@@ -4558,32 +4799,32 @@
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
       <c r="F86" s="3">
-        <v>5387434959</v>
+        <v>0</v>
       </c>
       <c r="G86" s="3">
-        <v>0</v>
+        <v>-26002382</v>
       </c>
       <c r="H86" s="3"/>
       <c r="I86" s="3"/>
       <c r="J86" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K86" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L86" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M86" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>273</v>
@@ -4591,7 +4832,7 @@
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
       <c r="F87" s="3">
-        <v>4749752753</v>
+        <v>5387434959</v>
       </c>
       <c r="G87" s="3">
         <v>0</v>
@@ -4599,24 +4840,24 @@
       <c r="H87" s="3"/>
       <c r="I87" s="3"/>
       <c r="J87" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L87" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M87" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>273</v>
@@ -4624,7 +4865,7 @@
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
       <c r="F88" s="3">
-        <v>637682206</v>
+        <v>4749752753</v>
       </c>
       <c r="G88" s="3">
         <v>0</v>
@@ -4644,12 +4885,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>273</v>
@@ -4657,7 +4898,7 @@
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
       <c r="F89" s="3">
-        <v>0</v>
+        <v>637682206</v>
       </c>
       <c r="G89" s="3">
         <v>0</v>
@@ -4665,24 +4906,24 @@
       <c r="H89" s="3"/>
       <c r="I89" s="3"/>
       <c r="J89" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K89" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L89" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M89" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>273</v>
@@ -4690,7 +4931,7 @@
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
       <c r="F90" s="3">
-        <v>4853244</v>
+        <v>0</v>
       </c>
       <c r="G90" s="3">
         <v>0</v>
@@ -4698,24 +4939,24 @@
       <c r="H90" s="3"/>
       <c r="I90" s="3"/>
       <c r="J90" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K90" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L90" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M90" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>273</v>
@@ -4723,7 +4964,7 @@
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
       <c r="F91" s="3">
-        <v>0</v>
+        <v>4853244</v>
       </c>
       <c r="G91" s="3">
         <v>0</v>
@@ -4731,24 +4972,24 @@
       <c r="H91" s="3"/>
       <c r="I91" s="3"/>
       <c r="J91" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K91" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L91" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M91" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>273</v>
@@ -4764,24 +5005,24 @@
       <c r="H92" s="3"/>
       <c r="I92" s="3"/>
       <c r="J92" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K92" s="1">
         <v>0</v>
       </c>
       <c r="L92" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M92" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>273</v>
@@ -4789,7 +5030,7 @@
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
       <c r="F93" s="3">
-        <v>385354183</v>
+        <v>0</v>
       </c>
       <c r="G93" s="3">
         <v>0</v>
@@ -4800,21 +5041,21 @@
         <v>0</v>
       </c>
       <c r="K93" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L93" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M93" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>273</v>
@@ -4822,7 +5063,7 @@
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
       <c r="F94" s="3">
-        <v>-653330658</v>
+        <v>385354183</v>
       </c>
       <c r="G94" s="3">
         <v>0</v>
@@ -4842,12 +5083,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>273</v>
@@ -4855,7 +5096,7 @@
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
       <c r="F95" s="3">
-        <v>85483250</v>
+        <v>-653330658</v>
       </c>
       <c r="G95" s="3">
         <v>0</v>
@@ -4875,12 +5116,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>273</v>
@@ -4888,7 +5129,7 @@
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
       <c r="F96" s="3">
-        <v>341600000</v>
+        <v>85483250</v>
       </c>
       <c r="G96" s="3">
         <v>0</v>
@@ -4908,12 +5149,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>273</v>
@@ -4921,7 +5162,7 @@
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
       <c r="F97" s="3">
-        <v>537899390</v>
+        <v>341600000</v>
       </c>
       <c r="G97" s="3">
         <v>0</v>
@@ -4941,12 +5182,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>273</v>
@@ -4954,7 +5195,7 @@
       <c r="D98" s="3"/>
       <c r="E98" s="3"/>
       <c r="F98" s="3">
-        <v>99204446</v>
+        <v>537899390</v>
       </c>
       <c r="G98" s="3">
         <v>0</v>
@@ -4968,18 +5209,18 @@
         <v>1</v>
       </c>
       <c r="L98" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M98" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>273</v>
@@ -4987,7 +5228,7 @@
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
       <c r="F99" s="3">
-        <v>0</v>
+        <v>99204446</v>
       </c>
       <c r="G99" s="3">
         <v>0</v>
@@ -4998,7 +5239,7 @@
         <v>0</v>
       </c>
       <c r="K99" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L99" s="1">
         <v>2</v>
@@ -5007,12 +5248,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>273</v>
@@ -5020,7 +5261,7 @@
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
       <c r="F100" s="3">
-        <v>4914996</v>
+        <v>0</v>
       </c>
       <c r="G100" s="3">
         <v>0</v>
@@ -5031,21 +5272,21 @@
         <v>0</v>
       </c>
       <c r="K100" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L100" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M100" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>164</v>
+        <v>197</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>273</v>
@@ -5053,7 +5294,7 @@
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
       <c r="F101" s="3">
-        <v>0</v>
+        <v>4914996</v>
       </c>
       <c r="G101" s="3">
         <v>0</v>
@@ -5064,21 +5305,21 @@
         <v>0</v>
       </c>
       <c r="K101" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L101" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M101" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>200</v>
+        <v>164</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>273</v>
@@ -5086,7 +5327,7 @@
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
       <c r="F102" s="3">
-        <v>243226195</v>
+        <v>0</v>
       </c>
       <c r="G102" s="3">
         <v>0</v>
@@ -5097,21 +5338,21 @@
         <v>0</v>
       </c>
       <c r="K102" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L102" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M102" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>273</v>
@@ -5119,7 +5360,7 @@
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>
       <c r="F103" s="3">
-        <v>181834032</v>
+        <v>243226195</v>
       </c>
       <c r="G103" s="3">
         <v>0</v>
@@ -5139,12 +5380,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>273</v>
@@ -5152,7 +5393,7 @@
       <c r="D104" s="3"/>
       <c r="E104" s="3"/>
       <c r="F104" s="3">
-        <v>240187181</v>
+        <v>181834032</v>
       </c>
       <c r="G104" s="3">
         <v>0</v>
@@ -5172,12 +5413,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>273</v>
@@ -5185,7 +5426,7 @@
       <c r="D105" s="3"/>
       <c r="E105" s="3"/>
       <c r="F105" s="3">
-        <v>12330663</v>
+        <v>240187181</v>
       </c>
       <c r="G105" s="3">
         <v>0</v>
@@ -5205,12 +5446,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>273</v>
@@ -5218,7 +5459,7 @@
       <c r="D106" s="3"/>
       <c r="E106" s="3"/>
       <c r="F106" s="3">
-        <v>89308459</v>
+        <v>12330663</v>
       </c>
       <c r="G106" s="3">
         <v>0</v>
@@ -5238,12 +5479,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>166</v>
+        <v>208</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>273</v>
@@ -5251,7 +5492,7 @@
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
       <c r="F107" s="3">
-        <v>0</v>
+        <v>89308459</v>
       </c>
       <c r="G107" s="3">
         <v>0</v>
@@ -5262,21 +5503,21 @@
         <v>0</v>
       </c>
       <c r="K107" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L107" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M107" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>273</v>
@@ -5284,7 +5525,7 @@
       <c r="D108" s="3"/>
       <c r="E108" s="3"/>
       <c r="F108" s="3">
-        <v>26630000</v>
+        <v>0</v>
       </c>
       <c r="G108" s="3">
         <v>0</v>
@@ -5295,21 +5536,21 @@
         <v>0</v>
       </c>
       <c r="K108" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L108" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M108" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>212</v>
+        <v>167</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>273</v>
@@ -5317,7 +5558,7 @@
       <c r="D109" s="3"/>
       <c r="E109" s="3"/>
       <c r="F109" s="3">
-        <v>51973310</v>
+        <v>26630000</v>
       </c>
       <c r="G109" s="3">
         <v>0</v>
@@ -5337,12 +5578,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>273</v>
@@ -5350,7 +5591,7 @@
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
       <c r="F110" s="3">
-        <v>10341004</v>
+        <v>51973310</v>
       </c>
       <c r="G110" s="3">
         <v>0</v>
@@ -5370,12 +5611,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>273</v>
@@ -5383,7 +5624,7 @@
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
       <c r="F111" s="3">
-        <v>0</v>
+        <v>10341004</v>
       </c>
       <c r="G111" s="3">
         <v>0</v>
@@ -5391,24 +5632,24 @@
       <c r="H111" s="3"/>
       <c r="I111" s="3"/>
       <c r="J111" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K111" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L111" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M111" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>273</v>
@@ -5424,24 +5665,24 @@
       <c r="H112" s="3"/>
       <c r="I112" s="3"/>
       <c r="J112" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K112" s="1">
         <v>0</v>
       </c>
       <c r="L112" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M112" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>273</v>
@@ -5449,7 +5690,7 @@
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
       <c r="F113" s="3">
-        <v>-653330657</v>
+        <v>0</v>
       </c>
       <c r="G113" s="3">
         <v>0</v>
@@ -5460,21 +5701,21 @@
         <v>0</v>
       </c>
       <c r="K113" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L113" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M113" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>273</v>
@@ -5482,7 +5723,7 @@
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
       <c r="F114" s="3">
-        <v>341600000</v>
+        <v>-653330657</v>
       </c>
       <c r="G114" s="3">
         <v>0</v>
@@ -5502,12 +5743,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>273</v>
@@ -5515,7 +5756,7 @@
       <c r="D115" s="3"/>
       <c r="E115" s="3"/>
       <c r="F115" s="3">
-        <v>537899388</v>
+        <v>341600000</v>
       </c>
       <c r="G115" s="3">
         <v>0</v>
@@ -5535,12 +5776,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>273</v>
@@ -5548,7 +5789,7 @@
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
       <c r="F116" s="3">
-        <v>7314355</v>
+        <v>537899388</v>
       </c>
       <c r="G116" s="3">
         <v>0</v>
@@ -5562,18 +5803,18 @@
         <v>1</v>
       </c>
       <c r="L116" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M116" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>195</v>
+        <v>226</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>273</v>
@@ -5581,7 +5822,7 @@
       <c r="D117" s="3"/>
       <c r="E117" s="3"/>
       <c r="F117" s="3">
-        <v>0</v>
+        <v>7314355</v>
       </c>
       <c r="G117" s="3">
         <v>0</v>
@@ -5592,7 +5833,7 @@
         <v>0</v>
       </c>
       <c r="K117" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L117" s="1">
         <v>2</v>
@@ -5601,12 +5842,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>229</v>
+        <v>195</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>273</v>
@@ -5614,7 +5855,7 @@
       <c r="D118" s="3"/>
       <c r="E118" s="3"/>
       <c r="F118" s="3">
-        <v>4914996</v>
+        <v>0</v>
       </c>
       <c r="G118" s="3">
         <v>0</v>
@@ -5625,21 +5866,21 @@
         <v>0</v>
       </c>
       <c r="K118" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L118" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M118" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>273</v>
@@ -5647,7 +5888,7 @@
       <c r="D119" s="3"/>
       <c r="E119" s="3"/>
       <c r="F119" s="3">
-        <v>3000000</v>
+        <v>4914996</v>
       </c>
       <c r="G119" s="3">
         <v>0</v>
@@ -5661,18 +5902,18 @@
         <v>1</v>
       </c>
       <c r="L119" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M119" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>164</v>
+        <v>231</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>273</v>
@@ -5680,7 +5921,7 @@
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
       <c r="F120" s="3">
-        <v>0</v>
+        <v>3000000</v>
       </c>
       <c r="G120" s="3">
         <v>0</v>
@@ -5691,7 +5932,7 @@
         <v>0</v>
       </c>
       <c r="K120" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L120" s="1">
         <v>2</v>
@@ -5700,12 +5941,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>234</v>
+        <v>164</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>273</v>
@@ -5713,7 +5954,7 @@
       <c r="D121" s="3"/>
       <c r="E121" s="3"/>
       <c r="F121" s="3">
-        <v>80181681</v>
+        <v>0</v>
       </c>
       <c r="G121" s="3">
         <v>0</v>
@@ -5724,21 +5965,21 @@
         <v>0</v>
       </c>
       <c r="K121" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L121" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M121" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>273</v>
@@ -5746,7 +5987,7 @@
       <c r="D122" s="3"/>
       <c r="E122" s="3"/>
       <c r="F122" s="3">
-        <v>227322131</v>
+        <v>80181681</v>
       </c>
       <c r="G122" s="3">
         <v>0</v>
@@ -5766,12 +6007,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>273</v>
@@ -5779,7 +6020,7 @@
       <c r="D123" s="3"/>
       <c r="E123" s="3"/>
       <c r="F123" s="3">
-        <v>595000</v>
+        <v>227322131</v>
       </c>
       <c r="G123" s="3">
         <v>0</v>
@@ -5799,12 +6040,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>273</v>
@@ -5812,7 +6053,7 @@
       <c r="D124" s="3"/>
       <c r="E124" s="3"/>
       <c r="F124" s="3">
-        <v>11775678</v>
+        <v>595000</v>
       </c>
       <c r="G124" s="3">
         <v>0</v>
@@ -5832,12 +6073,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>273</v>
@@ -5845,7 +6086,7 @@
       <c r="D125" s="3"/>
       <c r="E125" s="3"/>
       <c r="F125" s="3">
-        <v>27120000</v>
+        <v>11775678</v>
       </c>
       <c r="G125" s="3">
         <v>0</v>
@@ -5865,12 +6106,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>273</v>
@@ -5878,7 +6119,7 @@
       <c r="D126" s="3"/>
       <c r="E126" s="3"/>
       <c r="F126" s="3">
-        <v>35469098</v>
+        <v>27120000</v>
       </c>
       <c r="G126" s="3">
         <v>0</v>
@@ -5898,12 +6139,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>273</v>
@@ -5911,7 +6152,7 @@
       <c r="D127" s="3"/>
       <c r="E127" s="3"/>
       <c r="F127" s="3">
-        <v>32922041</v>
+        <v>35469098</v>
       </c>
       <c r="G127" s="3">
         <v>0</v>
@@ -5931,12 +6172,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>273</v>
@@ -5944,7 +6185,7 @@
       <c r="D128" s="3"/>
       <c r="E128" s="3"/>
       <c r="F128" s="3">
-        <v>1462963</v>
+        <v>32922041</v>
       </c>
       <c r="G128" s="3">
         <v>0</v>
@@ -5964,12 +6205,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>166</v>
+        <v>248</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>273</v>
@@ -5977,7 +6218,7 @@
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>
       <c r="F129" s="3">
-        <v>38500248</v>
+        <v>1462963</v>
       </c>
       <c r="G129" s="3">
         <v>0</v>
@@ -5991,18 +6232,18 @@
         <v>1</v>
       </c>
       <c r="L129" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M129" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>251</v>
+        <v>166</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>273</v>
@@ -6010,32 +6251,32 @@
       <c r="D130" s="3"/>
       <c r="E130" s="3"/>
       <c r="F130" s="3">
-        <v>0</v>
+        <v>38500248</v>
       </c>
       <c r="G130" s="3">
-        <v>4084968</v>
+        <v>0</v>
       </c>
       <c r="H130" s="3"/>
       <c r="I130" s="3"/>
       <c r="J130" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K130" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L130" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M130" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>273</v>
@@ -6046,29 +6287,29 @@
         <v>0</v>
       </c>
       <c r="G131" s="3">
-        <v>3560668</v>
+        <v>4084968</v>
       </c>
       <c r="H131" s="3"/>
       <c r="I131" s="3"/>
       <c r="J131" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K131" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L131" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M131" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>273</v>
@@ -6079,7 +6320,7 @@
         <v>0</v>
       </c>
       <c r="G132" s="3">
-        <v>524300</v>
+        <v>3560668</v>
       </c>
       <c r="H132" s="3"/>
       <c r="I132" s="3"/>
@@ -6096,12 +6337,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>165</v>
+        <v>251</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>273</v>
@@ -6109,29 +6350,29 @@
       <c r="D133" s="3"/>
       <c r="E133" s="3"/>
       <c r="F133" s="3">
-        <v>76405356</v>
+        <v>0</v>
       </c>
       <c r="G133" s="3">
-        <v>0</v>
+        <v>524300</v>
       </c>
       <c r="H133" s="3"/>
       <c r="I133" s="3"/>
       <c r="J133" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K133" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L133" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M133" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>165</v>
@@ -6150,24 +6391,24 @@
       <c r="H134" s="3"/>
       <c r="I134" s="3"/>
       <c r="J134" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K134" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L134" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M134" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>258</v>
+        <v>165</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>273</v>
@@ -6175,7 +6416,7 @@
       <c r="D135" s="3"/>
       <c r="E135" s="3"/>
       <c r="F135" s="3">
-        <v>123407221</v>
+        <v>76405356</v>
       </c>
       <c r="G135" s="3">
         <v>0</v>
@@ -6183,24 +6424,24 @@
       <c r="H135" s="3"/>
       <c r="I135" s="3"/>
       <c r="J135" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K135" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L135" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M135" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>273</v>
@@ -6216,38 +6457,71 @@
       <c r="H136" s="3"/>
       <c r="I136" s="3"/>
       <c r="J136" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K136" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L136" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M136" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>273</v>
+      </c>
       <c r="D137" s="3"/>
       <c r="E137" s="3"/>
-      <c r="F137" s="3"/>
-      <c r="G137" s="3"/>
+      <c r="F137" s="3">
+        <v>123407221</v>
+      </c>
+      <c r="G137" s="3">
+        <v>0</v>
+      </c>
       <c r="H137" s="3"/>
       <c r="I137" s="3"/>
-    </row>
-    <row r="138" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B138" s="4"/>
-      <c r="C138" s="4"/>
-      <c r="D138" s="5"/>
-      <c r="E138" s="5"/>
-      <c r="F138" s="5"/>
-      <c r="G138" s="5"/>
-      <c r="H138" s="5"/>
-      <c r="I138" s="5"/>
+      <c r="J137" s="1">
+        <v>0</v>
+      </c>
+      <c r="K137" s="1">
+        <v>1</v>
+      </c>
+      <c r="L137" s="1">
+        <v>2</v>
+      </c>
+      <c r="M137" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D138" s="3"/>
+      <c r="E138" s="3"/>
+      <c r="F138" s="3"/>
+      <c r="G138" s="3"/>
+      <c r="H138" s="3"/>
+      <c r="I138" s="3"/>
+    </row>
+    <row r="139" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B139" s="4"/>
+      <c r="C139" s="4"/>
+      <c r="D139" s="5"/>
+      <c r="E139" s="5"/>
+      <c r="F139" s="5"/>
+      <c r="G139" s="5"/>
+      <c r="H139" s="5"/>
+      <c r="I139" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M136" xr:uid="{F67FFD85-9FD5-489C-9A0F-49D2F75178B7}"/>
+  <autoFilter ref="A1:M137" xr:uid="{F67FFD85-9FD5-489C-9A0F-49D2F75178B7}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
Add financial statement mapping and aggregation logic
Introduces code and notebook logic for normalizing trial balance data, mapping leaf accounts to financial statement codes using prefix matching, and aggregating results for export. Adds supporting Excel templates and output artifacts for balance sheet and income statement pivots.
</commit_message>
<xml_diff>
--- a/data/TB_2024.xlsx
+++ b/data/TB_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XA XUI - CVN\Documents\GitHub\Planning_Agent_NDD\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EA8657-EE38-424D-BA80-DD68E6532DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA291F4-7197-4B3B-9492-51A936C9F99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7784254E-2EFB-49AF-922A-1AA81A05D961}"/>
   </bookViews>
@@ -821,9 +821,6 @@
     <t>Chi phí thuế TNDN hiện hành</t>
   </si>
   <si>
-    <t>Account No</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -867,6 +864,9 @@
   </si>
   <si>
     <t>Trả trước cho người bán</t>
+  </si>
+  <si>
+    <t>account_id</t>
   </si>
 </sst>
 </file>
@@ -924,7 +924,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -932,6 +932,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1340,10 +1341,10 @@
   <dimension ref="A1:M139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C73" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E78" sqref="E78"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1358,41 +1359,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="6" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>271</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>0</v>
@@ -1406,7 +1407,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D2" s="3">
         <v>6605748426</v>
@@ -1447,7 +1448,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D3" s="3">
         <v>897868646</v>
@@ -1488,7 +1489,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D4" s="3">
         <v>897868646</v>
@@ -1529,7 +1530,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D5" s="3">
         <v>5707879780</v>
@@ -1570,7 +1571,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D6" s="3">
         <v>5707879780</v>
@@ -1611,7 +1612,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
@@ -1652,7 +1653,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
@@ -1693,7 +1694,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D9" s="3">
         <v>706266798</v>
@@ -1734,7 +1735,7 @@
         <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D10" s="3">
         <v>706266798</v>
@@ -1775,7 +1776,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D11" s="3">
         <v>706266798</v>
@@ -1816,7 +1817,7 @@
         <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D12" s="3">
         <v>124047295</v>
@@ -1857,7 +1858,7 @@
         <v>24</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D13" s="3">
         <v>124047295</v>
@@ -1898,7 +1899,7 @@
         <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D14" s="3">
         <v>0</v>
@@ -1939,7 +1940,7 @@
         <v>28</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D15" s="3">
         <v>124047295</v>
@@ -1980,7 +1981,7 @@
         <v>30</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D16" s="3">
         <v>257292807</v>
@@ -2021,7 +2022,7 @@
         <v>30</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D17" s="3">
         <v>257292807</v>
@@ -2062,7 +2063,7 @@
         <v>33</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D18" s="3">
         <v>257292807</v>
@@ -2103,7 +2104,7 @@
         <v>35</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D19" s="3">
         <v>0</v>
@@ -2144,7 +2145,7 @@
         <v>33</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D20" s="3">
         <v>257292807</v>
@@ -2185,7 +2186,7 @@
         <v>38</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D21" s="3">
         <v>123228000</v>
@@ -2226,7 +2227,7 @@
         <v>40</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D22" s="3">
         <v>0</v>
@@ -2267,7 +2268,7 @@
         <v>42</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D23" s="3">
         <v>0</v>
@@ -2308,7 +2309,7 @@
         <v>44</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D24" s="3">
         <v>0</v>
@@ -2349,7 +2350,7 @@
         <v>46</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D25" s="3">
         <v>0</v>
@@ -2390,7 +2391,7 @@
         <v>48</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D26" s="3">
         <v>39320000</v>
@@ -2431,7 +2432,7 @@
         <v>50</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D27" s="3">
         <v>39320000</v>
@@ -2472,7 +2473,7 @@
         <v>52</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D28" s="3">
         <v>0</v>
@@ -2513,7 +2514,7 @@
         <v>54</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D29" s="3">
         <v>0</v>
@@ -2554,7 +2555,7 @@
         <v>56</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D30" s="3">
         <v>0</v>
@@ -2595,7 +2596,7 @@
         <v>58</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D31" s="3">
         <v>117685490</v>
@@ -2636,7 +2637,7 @@
         <v>60</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D32" s="3">
         <v>101595093</v>
@@ -2677,7 +2678,7 @@
         <v>62</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D33" s="3">
         <v>0</v>
@@ -2718,7 +2719,7 @@
         <v>64</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D34" s="3">
         <v>101595093</v>
@@ -2759,7 +2760,7 @@
         <v>66</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D35" s="3">
         <v>16090397</v>
@@ -2800,7 +2801,7 @@
         <v>68</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D36" s="3">
         <v>10549745</v>
@@ -2841,7 +2842,7 @@
         <v>70</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D37" s="3">
         <v>5540652</v>
@@ -2882,7 +2883,7 @@
         <v>72</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D38" s="3">
         <v>148099200</v>
@@ -2923,7 +2924,7 @@
         <v>74</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D39" s="3">
         <v>148099200</v>
@@ -2964,7 +2965,7 @@
         <v>76</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D40" s="3">
         <v>91360</v>
@@ -3005,7 +3006,7 @@
         <v>78</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D41" s="3">
         <v>91360</v>
@@ -3046,7 +3047,7 @@
         <v>80</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D42" s="3">
         <v>91360</v>
@@ -3081,13 +3082,13 @@
     </row>
     <row r="43" spans="1:13" s="6" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>276</v>
-      </c>
       <c r="C43" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D43" s="3">
         <v>0</v>
@@ -3128,7 +3129,7 @@
         <v>82</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D44" s="3">
         <v>0</v>
@@ -3169,7 +3170,7 @@
         <v>84</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D45" s="3">
         <v>0</v>
@@ -3210,7 +3211,7 @@
         <v>86</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D46" s="3">
         <v>0</v>
@@ -3251,7 +3252,7 @@
         <v>88</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D47" s="3">
         <v>0</v>
@@ -3292,7 +3293,7 @@
         <v>90</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D48" s="3">
         <v>0</v>
@@ -3333,7 +3334,7 @@
         <v>92</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D49" s="3">
         <v>0</v>
@@ -3374,7 +3375,7 @@
         <v>94</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D50" s="3">
         <v>0</v>
@@ -3415,7 +3416,7 @@
         <v>96</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D51" s="3">
         <v>0</v>
@@ -3456,7 +3457,7 @@
         <v>98</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D52" s="3">
         <v>0</v>
@@ -3497,7 +3498,7 @@
         <v>100</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D53" s="3">
         <v>0</v>
@@ -3538,7 +3539,7 @@
         <v>102</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D54" s="3">
         <v>0</v>
@@ -3579,7 +3580,7 @@
         <v>104</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D55" s="3">
         <v>0</v>
@@ -3620,7 +3621,7 @@
         <v>106</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D56" s="3">
         <v>0</v>
@@ -3661,7 +3662,7 @@
         <v>108</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D57" s="3">
         <v>0</v>
@@ -3702,7 +3703,7 @@
         <v>110</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D58" s="3">
         <v>0</v>
@@ -3743,7 +3744,7 @@
         <v>112</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D59" s="3">
         <v>0</v>
@@ -3784,7 +3785,7 @@
         <v>112</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D60" s="3">
         <v>0</v>
@@ -3825,7 +3826,7 @@
         <v>115</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D61" s="3">
         <v>0</v>
@@ -3866,7 +3867,7 @@
         <v>117</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D62" s="3">
         <v>0</v>
@@ -3907,7 +3908,7 @@
         <v>119</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D63" s="3">
         <v>0</v>
@@ -3948,7 +3949,7 @@
         <v>121</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D64" s="3">
         <v>0</v>
@@ -3989,7 +3990,7 @@
         <v>123</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D65" s="3">
         <v>0</v>
@@ -4030,7 +4031,7 @@
         <v>125</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D66" s="3">
         <v>0</v>
@@ -4071,7 +4072,7 @@
         <v>127</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D67" s="3">
         <v>0</v>
@@ -4112,7 +4113,7 @@
         <v>129</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D68" s="3">
         <v>0</v>
@@ -4153,7 +4154,7 @@
         <v>121</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D69" s="3">
         <v>0</v>
@@ -4194,7 +4195,7 @@
         <v>132</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D70" s="3">
         <v>0</v>
@@ -4235,7 +4236,7 @@
         <v>132</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D71" s="3">
         <v>0</v>
@@ -4276,7 +4277,7 @@
         <v>135</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D72" s="3">
         <v>0</v>
@@ -4317,7 +4318,7 @@
         <v>137</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D73" s="3">
         <v>0</v>
@@ -4358,7 +4359,7 @@
         <v>139</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D74" s="3">
         <v>0</v>
@@ -4399,7 +4400,7 @@
         <v>141</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D75" s="3">
         <v>0</v>
@@ -4440,7 +4441,7 @@
         <v>143</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D76" s="3">
         <v>6290591391</v>
@@ -4481,7 +4482,7 @@
         <v>145</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D77" s="3">
         <v>4171107126</v>
@@ -4522,7 +4523,7 @@
         <v>147</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D78" s="3">
         <v>2119484265</v>
@@ -4563,7 +4564,7 @@
         <v>149</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
@@ -4596,7 +4597,7 @@
         <v>151</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
@@ -4629,7 +4630,7 @@
         <v>153</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
@@ -4662,7 +4663,7 @@
         <v>155</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
@@ -4695,7 +4696,7 @@
         <v>157</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
@@ -4728,7 +4729,7 @@
         <v>159</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
@@ -4761,7 +4762,7 @@
         <v>161</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
@@ -4794,7 +4795,7 @@
         <v>163</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
@@ -4827,7 +4828,7 @@
         <v>169</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
@@ -4860,7 +4861,7 @@
         <v>171</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
@@ -4893,7 +4894,7 @@
         <v>173</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
@@ -4926,7 +4927,7 @@
         <v>175</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
@@ -4959,7 +4960,7 @@
         <v>177</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
@@ -4992,7 +4993,7 @@
         <v>179</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
@@ -5025,7 +5026,7 @@
         <v>181</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
@@ -5058,7 +5059,7 @@
         <v>183</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
@@ -5091,7 +5092,7 @@
         <v>185</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
@@ -5124,7 +5125,7 @@
         <v>187</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D96" s="3"/>
       <c r="E96" s="3"/>
@@ -5157,7 +5158,7 @@
         <v>189</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
@@ -5190,7 +5191,7 @@
         <v>191</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D98" s="3"/>
       <c r="E98" s="3"/>
@@ -5223,7 +5224,7 @@
         <v>193</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
@@ -5256,7 +5257,7 @@
         <v>195</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
@@ -5289,7 +5290,7 @@
         <v>197</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
@@ -5322,7 +5323,7 @@
         <v>164</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
@@ -5355,7 +5356,7 @@
         <v>200</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>
@@ -5388,7 +5389,7 @@
         <v>202</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D104" s="3"/>
       <c r="E104" s="3"/>
@@ -5421,7 +5422,7 @@
         <v>204</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D105" s="3"/>
       <c r="E105" s="3"/>
@@ -5454,7 +5455,7 @@
         <v>206</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D106" s="3"/>
       <c r="E106" s="3"/>
@@ -5487,7 +5488,7 @@
         <v>208</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
@@ -5520,7 +5521,7 @@
         <v>166</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D108" s="3"/>
       <c r="E108" s="3"/>
@@ -5553,7 +5554,7 @@
         <v>167</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D109" s="3"/>
       <c r="E109" s="3"/>
@@ -5586,7 +5587,7 @@
         <v>212</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
@@ -5619,7 +5620,7 @@
         <v>214</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
@@ -5652,7 +5653,7 @@
         <v>216</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D112" s="3"/>
       <c r="E112" s="3"/>
@@ -5685,7 +5686,7 @@
         <v>218</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
@@ -5718,7 +5719,7 @@
         <v>220</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
@@ -5751,7 +5752,7 @@
         <v>222</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D115" s="3"/>
       <c r="E115" s="3"/>
@@ -5784,7 +5785,7 @@
         <v>224</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
@@ -5817,7 +5818,7 @@
         <v>226</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D117" s="3"/>
       <c r="E117" s="3"/>
@@ -5850,7 +5851,7 @@
         <v>195</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D118" s="3"/>
       <c r="E118" s="3"/>
@@ -5883,7 +5884,7 @@
         <v>229</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D119" s="3"/>
       <c r="E119" s="3"/>
@@ -5916,7 +5917,7 @@
         <v>231</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
@@ -5949,7 +5950,7 @@
         <v>164</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D121" s="3"/>
       <c r="E121" s="3"/>
@@ -5982,7 +5983,7 @@
         <v>234</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D122" s="3"/>
       <c r="E122" s="3"/>
@@ -6015,7 +6016,7 @@
         <v>236</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D123" s="3"/>
       <c r="E123" s="3"/>
@@ -6048,7 +6049,7 @@
         <v>238</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D124" s="3"/>
       <c r="E124" s="3"/>
@@ -6081,7 +6082,7 @@
         <v>240</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D125" s="3"/>
       <c r="E125" s="3"/>
@@ -6114,7 +6115,7 @@
         <v>242</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D126" s="3"/>
       <c r="E126" s="3"/>
@@ -6147,7 +6148,7 @@
         <v>244</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D127" s="3"/>
       <c r="E127" s="3"/>
@@ -6180,7 +6181,7 @@
         <v>246</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D128" s="3"/>
       <c r="E128" s="3"/>
@@ -6213,7 +6214,7 @@
         <v>248</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>
@@ -6246,7 +6247,7 @@
         <v>166</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D130" s="3"/>
       <c r="E130" s="3"/>
@@ -6279,7 +6280,7 @@
         <v>251</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D131" s="3"/>
       <c r="E131" s="3"/>
@@ -6312,7 +6313,7 @@
         <v>253</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D132" s="3"/>
       <c r="E132" s="3"/>
@@ -6345,7 +6346,7 @@
         <v>251</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D133" s="3"/>
       <c r="E133" s="3"/>
@@ -6378,7 +6379,7 @@
         <v>165</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D134" s="3"/>
       <c r="E134" s="3"/>
@@ -6411,7 +6412,7 @@
         <v>165</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D135" s="3"/>
       <c r="E135" s="3"/>
@@ -6444,7 +6445,7 @@
         <v>258</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D136" s="3"/>
       <c r="E136" s="3"/>
@@ -6477,7 +6478,7 @@
         <v>260</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D137" s="3"/>
       <c r="E137" s="3"/>

</xml_diff>